<commit_message>
Add convolution between shutter and light to the Photonic Class
</commit_message>
<xml_diff>
--- a/data/photonic_simul_data.xlsx
+++ b/data/photonic_simul_data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -133,12 +133,36 @@
     <t>BurstTime_s</t>
   </si>
   <si>
+    <t>light_rise_sec</t>
+  </si>
+  <si>
+    <t>light_fall_sec</t>
+  </si>
+  <si>
+    <t>light_width_sec</t>
+  </si>
+  <si>
+    <t>shutter_rise_sec</t>
+  </si>
+  <si>
+    <t>shutter_fall_sec</t>
+  </si>
+  <si>
+    <t>shutter_width_sec</t>
+  </si>
+  <si>
+    <t>shutter_delay_sec</t>
+  </si>
+  <si>
     <t>CW_30fps</t>
   </si>
   <si>
     <t>CW_60fps</t>
   </si>
   <si>
+    <t>pls_30_1000</t>
+  </si>
+  <si>
     <t>Config</t>
   </si>
   <si>
@@ -146,15 +170,20 @@
   </si>
   <si>
     <t>Cfg2</t>
+  </si>
+  <si>
+    <t>Cfg3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="0.0######E+00"/>
+    <numFmt numFmtId="60" formatCode="0.0########E+00"/>
+    <numFmt numFmtId="61" formatCode="0.0#######E+00"/>
   </numFmts>
   <fonts count="7">
     <font>
@@ -472,7 +501,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -582,6 +611,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1803,7 +1841,7 @@
     </row>
     <row r="19">
       <c r="B19" t="s" s="3">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
@@ -1814,7 +1852,7 @@
         <v>5</v>
       </c>
       <c r="D20" t="s" s="5">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -2403,7 +2441,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E11"/>
+  <dimension ref="A2:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
       <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
@@ -2411,8 +2449,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="36" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="36" customWidth="1"/>
+    <col min="1" max="12" width="16.3516" style="36" customWidth="1"/>
+    <col min="13" max="16384" width="16.3516" style="36" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
@@ -2423,6 +2461,13 @@
       <c r="C1" s="7"/>
       <c r="D1" s="7"/>
       <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
     </row>
     <row r="2" ht="20.45" customHeight="1">
       <c r="A2" t="s" s="8">
@@ -2437,13 +2482,34 @@
       <c r="D2" t="s" s="9">
         <v>36</v>
       </c>
-      <c r="E2" t="s" s="10">
+      <c r="E2" t="s" s="9">
         <v>37</v>
+      </c>
+      <c r="F2" t="s" s="9">
+        <v>38</v>
+      </c>
+      <c r="G2" t="s" s="9">
+        <v>39</v>
+      </c>
+      <c r="H2" t="s" s="9">
+        <v>40</v>
+      </c>
+      <c r="I2" t="s" s="9">
+        <v>41</v>
+      </c>
+      <c r="J2" t="s" s="9">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s" s="9">
+        <v>43</v>
+      </c>
+      <c r="L2" t="s" s="10">
+        <v>44</v>
       </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="11">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="B3" s="12">
         <v>30</v>
@@ -2454,14 +2520,21 @@
       <c r="D3" s="13">
         <v>0.0036</v>
       </c>
-      <c r="E3" s="14">
-        <f>1/B3</f>
-        <v>0.0333333333333333</v>
-      </c>
+      <c r="E3" s="13">
+        <f>1/B3/2</f>
+        <v>0.0166666666666667</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+      <c r="L3" s="29"/>
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="15">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B4" s="16">
         <v>60</v>
@@ -2472,63 +2545,144 @@
       <c r="D4" s="17">
         <v>0.5</v>
       </c>
-      <c r="E4" s="18">
-        <f>1/B4</f>
-        <v>0.0166666666666667</v>
-      </c>
+      <c r="E4" s="17">
+        <f>1/B4/2</f>
+        <v>0.00833333333333333</v>
+      </c>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
+      <c r="A5" t="s" s="15">
+        <v>47</v>
+      </c>
+      <c r="B5" s="16">
+        <v>30</v>
+      </c>
+      <c r="C5" s="17">
+        <v>1000</v>
+      </c>
+      <c r="D5" s="17">
+        <v>0.0036</v>
+      </c>
+      <c r="E5" s="17">
+        <f>1/B5/10</f>
+        <v>0.00333333333333333</v>
+      </c>
+      <c r="F5" s="37">
+        <v>3e-09</v>
+      </c>
+      <c r="G5" s="37">
+        <v>5e-09</v>
+      </c>
+      <c r="H5" s="38">
+        <v>1e-08</v>
+      </c>
+      <c r="I5" s="37">
+        <v>1e-09</v>
+      </c>
+      <c r="J5" s="37">
+        <v>1e-09</v>
+      </c>
+      <c r="K5" s="38">
+        <v>1e-08</v>
+      </c>
+      <c r="L5" s="39">
+        <v>3e-09</v>
+      </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
       <c r="A6" s="19"/>
       <c r="B6" s="20"/>
       <c r="C6" s="21"/>
       <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="22"/>
     </row>
     <row r="7" ht="20.2" customHeight="1">
       <c r="A7" s="19"/>
       <c r="B7" s="20"/>
       <c r="C7" s="21"/>
       <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="22"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
       <c r="C8" s="21"/>
       <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="22"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
       <c r="A9" s="19"/>
       <c r="B9" s="20"/>
       <c r="C9" s="21"/>
       <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="22"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
       <c r="A10" s="19"/>
       <c r="B10" s="20"/>
       <c r="C10" s="21"/>
       <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="22"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
       <c r="A11" s="23"/>
       <c r="B11" s="24"/>
       <c r="C11" s="25"/>
       <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
+      <c r="I11" s="25"/>
+      <c r="J11" s="25"/>
+      <c r="K11" s="25"/>
+      <c r="L11" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A1:L1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -2551,8 +2705,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="37" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="37" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="40" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="40" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
@@ -2587,51 +2741,63 @@
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="11">
-        <v>41</v>
-      </c>
-      <c r="B3" t="s" s="38">
+        <v>49</v>
+      </c>
+      <c r="B3" t="s" s="41">
         <v>12</v>
       </c>
-      <c r="C3" t="s" s="39">
+      <c r="C3" t="s" s="42">
         <v>18</v>
       </c>
-      <c r="D3" t="s" s="39">
+      <c r="D3" t="s" s="42">
         <v>22</v>
       </c>
-      <c r="E3" t="s" s="40">
+      <c r="E3" t="s" s="43">
         <v>31</v>
       </c>
-      <c r="F3" t="s" s="41">
-        <v>38</v>
+      <c r="F3" t="s" s="44">
+        <v>45</v>
       </c>
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="15">
-        <v>42</v>
-      </c>
-      <c r="B4" t="s" s="42">
+        <v>50</v>
+      </c>
+      <c r="B4" t="s" s="45">
         <v>13</v>
       </c>
-      <c r="C4" t="s" s="43">
+      <c r="C4" t="s" s="46">
         <v>18</v>
       </c>
-      <c r="D4" t="s" s="43">
+      <c r="D4" t="s" s="46">
         <v>23</v>
       </c>
-      <c r="E4" t="s" s="44">
+      <c r="E4" t="s" s="47">
         <v>32</v>
       </c>
-      <c r="F4" t="s" s="45">
-        <v>39</v>
+      <c r="F4" t="s" s="48">
+        <v>46</v>
       </c>
     </row>
     <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22"/>
+      <c r="A5" t="s" s="15">
+        <v>51</v>
+      </c>
+      <c r="B5" t="s" s="45">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s" s="46">
+        <v>18</v>
+      </c>
+      <c r="D5" t="s" s="46">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s" s="47">
+        <v>31</v>
+      </c>
+      <c r="F5" t="s" s="48">
+        <v>47</v>
+      </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
       <c r="A6" s="19"/>

</xml_diff>

<commit_message>
Now QE is calc by absorption coefficient and epitaxial semiconductor layer thichness
</commit_message>
<xml_diff>
--- a/data/photonic_simul_data.xlsx
+++ b/data/photonic_simul_data.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -31,10 +31,97 @@
     <t>Excel Worksheet Name</t>
   </si>
   <si>
+    <t>Export Summary</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
     <t>Light</t>
   </si>
   <si>
-    <t>Table 1</t>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Light</t>
+    </r>
+  </si>
+  <si>
+    <t>Scene</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Scene</t>
+    </r>
+  </si>
+  <si>
+    <t>Lens</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Lens</t>
+    </r>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Sensor</t>
+    </r>
+  </si>
+  <si>
+    <t>Op</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Op</t>
+    </r>
+  </si>
+  <si>
+    <t>Config</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="12"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Config</t>
+    </r>
+  </si>
+  <si>
+    <t>Light Table</t>
   </si>
   <si>
     <t>Name</t>
@@ -55,13 +142,82 @@
     <t>Vfov_deg</t>
   </si>
   <si>
+    <t>Number_units</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>Voltage_V</t>
+  </si>
+  <si>
+    <t>Current_A</t>
+  </si>
+  <si>
     <t>Laser1</t>
   </si>
   <si>
     <t>VCSEL2</t>
   </si>
   <si>
-    <t>Scene</t>
+    <t>L1550G1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.thorlabs.com/drawings/471c86010a0aa6dc-F53DE964-0AE3-E9AF-406B86F1AA7C426E/L1550G1-SpecSheet.pdf</t>
+    </r>
+  </si>
+  <si>
+    <t>MCM-105</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf</t>
+    </r>
+  </si>
+  <si>
+    <t>VCSEL_940_ii_vi</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.ii-vi.com/wp-content/uploads/2019/07/940nm-Multi-Mode-High-Power-VCSEL-Array-web-2-1.pdf</t>
+    </r>
+  </si>
+  <si>
+    <t>MCM-124</t>
+  </si>
+  <si>
+    <t>fake_tof_850</t>
+  </si>
+  <si>
+    <t>fake_tof_940</t>
+  </si>
+  <si>
+    <t>fake_tof_1375</t>
+  </si>
+  <si>
+    <t>fake_tof_1550</t>
+  </si>
+  <si>
+    <t>Scenario Table</t>
   </si>
   <si>
     <t>Distance_m</t>
@@ -73,25 +229,43 @@
     <t>AmbientLight_lux</t>
   </si>
   <si>
-    <t>Room</t>
-  </si>
-  <si>
-    <t>Road_Day</t>
-  </si>
-  <si>
-    <t>Lens</t>
+    <t>Room_3</t>
+  </si>
+  <si>
+    <t>Road_Day_60</t>
+  </si>
+  <si>
+    <t>Road_night_200</t>
+  </si>
+  <si>
+    <t>Outdoor_5</t>
+  </si>
+  <si>
+    <t>Room_5</t>
+  </si>
+  <si>
+    <t>Lens Table</t>
   </si>
   <si>
     <t>F_num</t>
   </si>
   <si>
+    <t>focal_length_m</t>
+  </si>
+  <si>
+    <t>BP_filter_width_nm</t>
+  </si>
+  <si>
     <t>Lens1</t>
   </si>
   <si>
     <t>Lens2</t>
   </si>
   <si>
-    <t>Sensor</t>
+    <t>fake_tof_lens</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensor Table </t>
   </si>
   <si>
     <t>PixelSize_m</t>
@@ -100,6 +274,12 @@
     <t>Wavelength</t>
   </si>
   <si>
+    <t>Semiconductor</t>
+  </si>
+  <si>
+    <t>epi_thick_um</t>
+  </si>
+  <si>
     <t>QE</t>
   </si>
   <si>
@@ -112,13 +292,43 @@
     <t>ArrayRes_V</t>
   </si>
   <si>
+    <t>ReadoutNoise_e</t>
+  </si>
+  <si>
+    <t>DarkSignal_e_s</t>
+  </si>
+  <si>
+    <t>Cfd_farad</t>
+  </si>
+  <si>
+    <t>CDS</t>
+  </si>
+  <si>
     <t>Sensor1_850</t>
   </si>
   <si>
+    <t>Si</t>
+  </si>
+  <si>
     <t>Sensor1_550</t>
   </si>
   <si>
-    <t>Op</t>
+    <t>ToF_850</t>
+  </si>
+  <si>
+    <t>ToF_940</t>
+  </si>
+  <si>
+    <t>ToF_1375</t>
+  </si>
+  <si>
+    <t>Ge</t>
+  </si>
+  <si>
+    <t>ToF_1550</t>
+  </si>
+  <si>
+    <t>Operational Modes Table</t>
   </si>
   <si>
     <t>frame_rate</t>
@@ -163,7 +373,10 @@
     <t>pls_30_1000</t>
   </si>
   <si>
-    <t>Config</t>
+    <t>fake_tof</t>
+  </si>
+  <si>
+    <t>Configurations Table</t>
   </si>
   <si>
     <t>Cfg1</t>
@@ -172,20 +385,50 @@
     <t>Cfg2</t>
   </si>
   <si>
+    <t>Room_4</t>
+  </si>
+  <si>
     <t>Cfg3</t>
+  </si>
+  <si>
+    <t>fake_tof_night_850</t>
+  </si>
+  <si>
+    <t>fake_tof_night_940</t>
+  </si>
+  <si>
+    <t>fake_tof_night_1375</t>
+  </si>
+  <si>
+    <t>fake_tof_night_1550</t>
+  </si>
+  <si>
+    <t>fake_tof_day_850</t>
+  </si>
+  <si>
+    <t>fake_tof_day_940</t>
+  </si>
+  <si>
+    <t>fake_tof_day_1375</t>
+  </si>
+  <si>
+    <t>fake_tof_day_1550</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="7">
     <numFmt numFmtId="0" formatCode="General"/>
-    <numFmt numFmtId="59" formatCode="0.0######E+00"/>
-    <numFmt numFmtId="60" formatCode="0.0########E+00"/>
-    <numFmt numFmtId="61" formatCode="0.0#######E+00"/>
+    <numFmt numFmtId="59" formatCode="0.0##E+00"/>
+    <numFmt numFmtId="60" formatCode="0.0?#####E+00"/>
+    <numFmt numFmtId="61" formatCode="0.0######E+00"/>
+    <numFmt numFmtId="62" formatCode="0.0#############E+00"/>
+    <numFmt numFmtId="63" formatCode="0.0?#######E+00"/>
+    <numFmt numFmtId="64" formatCode="0.0?######E+00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -213,6 +456,11 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
       <b val="1"/>
       <sz val="10"/>
       <color indexed="8"/>
@@ -223,8 +471,14 @@
       <color indexed="8"/>
       <name val="Helvetica Neue Medium"/>
     </font>
+    <font>
+      <u val="single"/>
+      <sz val="10"/>
+      <color indexed="12"/>
+      <name val="Helvetica Neue"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -245,24 +499,36 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor indexed="14"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="15"/>
+        <bgColor auto="1"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor indexed="10"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="13"/>
+        <fgColor indexed="17"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor indexed="16"/>
+        <fgColor indexed="19"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -272,13 +538,137 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="13"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="13"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -287,13 +677,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -302,13 +692,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </top>
       <bottom style="thin">
         <color indexed="8"/>
@@ -317,7 +707,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
@@ -326,7 +716,7 @@
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
@@ -335,58 +725,58 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
         <color indexed="8"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
@@ -395,58 +785,103 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
       </left>
       <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
@@ -455,43 +890,188 @@
         <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </left>
       <right style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </left>
       <right style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="15"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="14"/>
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="13"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="13"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="18"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="18"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="16"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="16"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="16"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
@@ -501,7 +1081,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -520,133 +1100,292 @@
     <xf numFmtId="0" fontId="4" fillId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="5" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="6" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="59" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="61" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="60" fontId="0" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="7" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="22" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="27" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="30" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="31" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="32" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="33" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="34" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="6" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="21" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="28" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="59" fontId="0" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="60" fontId="0" fillId="6" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="0" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="62" fontId="0" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="0" fillId="6" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="62" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="63" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="64" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="63" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -670,8 +1409,11 @@
       <rgbColor rgb="ff000000"/>
       <rgbColor rgb="01eef3f4"/>
       <rgbColor rgb="ff0000ff"/>
+      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ff5e88b1"/>
+      <rgbColor rgb="ffeef3f4"/>
+      <rgbColor rgb="ffafafaf"/>
       <rgbColor rgb="ff434443"/>
-      <rgbColor rgb="ffafafaf"/>
       <rgbColor rgb="ffb5b5b5"/>
       <rgbColor rgb="ff2c2c2c"/>
     </indexedColors>
@@ -690,10 +1432,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="434343"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="A9A9A9"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="0076BA"/>
@@ -872,9 +1614,12 @@
         <a:solidFill>
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -883,7 +1628,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -898,7 +1643,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="2200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -907,10 +1652,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1160,10 +1905,10 @@
         <a:noFill/>
         <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="FFFFFF"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -1454,7 +2199,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1474,7 +2219,7 @@
               <a:noFill/>
             </a:ln>
             <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
+              <a:srgbClr val="000000"/>
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
@@ -1732,276 +2477,640 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10" defaultRowHeight="13" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="2" customWidth="1"/>
+    <col min="1" max="1" width="2" style="6" customWidth="1"/>
     <col min="2" max="4" width="33.6016" customWidth="1"/>
+    <col min="2" max="2" width="33.6719" style="6" customWidth="1"/>
+    <col min="3" max="3" width="33.6719" style="6" customWidth="1"/>
+    <col min="4" max="4" width="33.6719" style="6" customWidth="1"/>
+    <col min="5" max="5" width="10" style="6" customWidth="1"/>
+    <col min="6" max="16384" width="10" style="6" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" ht="14.7" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="9"/>
+    </row>
+    <row r="2" ht="14.7" customHeight="1">
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
     <row r="3" ht="50" customHeight="1">
-      <c r="B3" t="s" s="1">
+      <c r="A3" s="10"/>
+      <c r="B3" t="s" s="13">
         <v>0</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" ht="14.7" customHeight="1">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" ht="14.7" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" ht="14.7" customHeight="1">
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7">
-      <c r="B7" t="s" s="2">
+      <c r="A7" s="10"/>
+      <c r="B7" t="s" s="14">
         <v>1</v>
       </c>
-      <c r="C7" t="s" s="2">
+      <c r="C7" t="s" s="14">
         <v>2</v>
       </c>
-      <c r="D7" t="s" s="2">
+      <c r="D7" t="s" s="14">
         <v>3</v>
       </c>
+      <c r="E7" s="12"/>
+    </row>
+    <row r="8" ht="14.7" customHeight="1">
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9">
-      <c r="B9" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3"/>
+      <c r="A9" s="10"/>
+      <c r="B9" t="s" s="15">
+        <v>6</v>
+      </c>
+      <c r="C9" s="16"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="12"/>
     </row>
     <row r="10">
-      <c r="B10" s="4"/>
-      <c r="C10" t="s" s="4">
+      <c r="A10" s="10"/>
+      <c r="B10" s="17"/>
+      <c r="C10" t="s" s="18">
         <v>5</v>
       </c>
-      <c r="D10" t="s" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11">
+      <c r="D10" t="s" s="19">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+    </row>
+    <row r="11" ht="13" customHeight="1">
+      <c r="A11" s="10"/>
       <c r="B11" t="s" s="3">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-    </row>
-    <row r="12">
+      <c r="E11" s="12"/>
+    </row>
+    <row r="12" ht="13" customHeight="1">
+      <c r="A12" s="10"/>
       <c r="B12" s="4"/>
       <c r="C12" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D12" t="s" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13">
+        <v>6</v>
+      </c>
+      <c r="E12" s="12"/>
+    </row>
+    <row r="13" ht="13" customHeight="1">
+      <c r="A13" s="10"/>
       <c r="B13" t="s" s="3">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-    </row>
-    <row r="14">
+      <c r="E13" s="12"/>
+    </row>
+    <row r="14" ht="13" customHeight="1">
+      <c r="A14" s="10"/>
       <c r="B14" s="4"/>
       <c r="C14" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D14" t="s" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="15">
+        <v>8</v>
+      </c>
+      <c r="E14" s="12"/>
+    </row>
+    <row r="15" ht="13" customHeight="1">
+      <c r="A15" s="10"/>
       <c r="B15" t="s" s="3">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="C15" s="3"/>
       <c r="D15" s="3"/>
-    </row>
-    <row r="16">
+      <c r="E15" s="12"/>
+    </row>
+    <row r="16" ht="13" customHeight="1">
+      <c r="A16" s="10"/>
       <c r="B16" s="4"/>
       <c r="C16" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D16" t="s" s="5">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17">
+        <v>10</v>
+      </c>
+      <c r="E16" s="12"/>
+    </row>
+    <row r="17" ht="13" customHeight="1">
+      <c r="A17" s="10"/>
       <c r="B17" t="s" s="3">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
-    </row>
-    <row r="18">
+      <c r="E17" s="12"/>
+    </row>
+    <row r="18" ht="13" customHeight="1">
+      <c r="A18" s="10"/>
       <c r="B18" s="4"/>
       <c r="C18" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D18" t="s" s="5">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19">
+        <v>12</v>
+      </c>
+      <c r="E18" s="12"/>
+    </row>
+    <row r="19" ht="13" customHeight="1">
+      <c r="A19" s="10"/>
       <c r="B19" t="s" s="3">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-    </row>
-    <row r="20">
+      <c r="E19" s="12"/>
+    </row>
+    <row r="20" ht="13" customHeight="1">
+      <c r="A20" s="20"/>
       <c r="B20" s="4"/>
       <c r="C20" t="s" s="4">
         <v>5</v>
       </c>
       <c r="D20" t="s" s="5">
-        <v>48</v>
+        <v>14</v>
+      </c>
+      <c r="E20" s="24"/>
+    </row>
+    <row r="21">
+      <c r="B21" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22">
+      <c r="B22" s="4"/>
+      <c r="C22" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" t="s" s="5">
+        <v>16</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="B3:D3"/>
     <mergeCell ref="B3:D3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D10" location="'Light'!R2C1" tooltip="" display="Light"/>
-    <hyperlink ref="D12" location="'Scene'!R2C1" tooltip="" display="Scene"/>
-    <hyperlink ref="D14" location="'Lens'!R2C1" tooltip="" display="Lens"/>
-    <hyperlink ref="D16" location="'Sensor'!R2C1" tooltip="" display="Sensor"/>
-    <hyperlink ref="D18" location="'Op'!R2C1" tooltip="" display="Op"/>
-    <hyperlink ref="D20" location="'Config'!R2C1" tooltip="" display="Config"/>
+    <hyperlink ref="D10" location="'Export Summary'!R1C1" tooltip="" display="Export Summary"/>
+    <hyperlink ref="D10" location="'Light'!R1C1" tooltip="" display="Light"/>
+    <hyperlink ref="D12" location="'Scene'!R1C1" tooltip="" display="Scene"/>
+    <hyperlink ref="D14" location="'Lens'!R1C1" tooltip="" display="Lens"/>
+    <hyperlink ref="D16" location="'Sensor'!R1C1" tooltip="" display="Sensor"/>
+    <hyperlink ref="D18" location="'Op'!R1C1" tooltip="" display="Op"/>
+    <hyperlink ref="D20" location="'Config'!R1C1" tooltip="" display="Config"/>
+    <hyperlink ref="D12" location="'Light'!R1C1" tooltip="" display="Light"/>
+    <hyperlink ref="D14" location="'Scene'!R1C1" tooltip="" display="Scene"/>
+    <hyperlink ref="D16" location="'Lens'!R1C1" tooltip="" display="Lens"/>
+    <hyperlink ref="D18" location="'Sensor'!R1C1" tooltip="" display="Sensor"/>
+    <hyperlink ref="D20" location="'Op'!R1C1" tooltip="" display="Op"/>
+    <hyperlink ref="D22" location="'Config'!R1C1" tooltip="" display="Config"/>
   </hyperlinks>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A2:F9"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="6" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="6" customWidth="1"/>
+    <col min="1" max="1" width="15.8594" style="25" customWidth="1"/>
+    <col min="2" max="2" width="10.1719" style="25" customWidth="1"/>
+    <col min="3" max="10" width="10.1172" style="25" customWidth="1"/>
+    <col min="11" max="16384" width="16.3516" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="8">
+      <c r="A1" s="26"/>
+      <c r="B1" s="27"/>
+      <c r="C1" t="s" s="28">
+        <v>18</v>
+      </c>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="30"/>
+    </row>
+    <row r="2" ht="26.7" customHeight="1">
+      <c r="A2" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="32">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s" s="32">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s" s="32">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s" s="32">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s" s="32">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s" s="32">
+        <v>25</v>
+      </c>
+      <c r="H2" t="s" s="32">
+        <v>26</v>
+      </c>
+      <c r="I2" t="s" s="32">
+        <v>27</v>
+      </c>
+      <c r="J2" t="s" s="33">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" ht="20.45" customHeight="1">
+      <c r="A3" t="s" s="34">
+        <v>29</v>
+      </c>
+      <c r="B3" s="35">
+        <v>20</v>
+      </c>
+      <c r="C3" s="36">
+        <v>850</v>
+      </c>
+      <c r="D3" s="36">
+        <v>0.95</v>
+      </c>
+      <c r="E3" s="36">
+        <v>60</v>
+      </c>
+      <c r="F3" s="36">
+        <v>60</v>
+      </c>
+      <c r="G3" s="36">
+        <v>1</v>
+      </c>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="38"/>
+    </row>
+    <row r="4" ht="20.2" customHeight="1">
+      <c r="A4" t="s" s="39">
+        <v>30</v>
+      </c>
+      <c r="B4" s="40">
+        <v>10</v>
+      </c>
+      <c r="C4" s="41">
+        <v>940</v>
+      </c>
+      <c r="D4" s="41">
+        <v>0.95</v>
+      </c>
+      <c r="E4" s="41">
+        <v>60</v>
+      </c>
+      <c r="F4" s="41">
+        <v>60</v>
+      </c>
+      <c r="G4" s="41">
+        <v>1</v>
+      </c>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="43"/>
+    </row>
+    <row r="5" ht="20.2" customHeight="1">
+      <c r="A5" t="s" s="39">
+        <v>31</v>
+      </c>
+      <c r="B5" s="40">
+        <v>2.1</v>
+      </c>
+      <c r="C5" s="41">
+        <v>1550</v>
+      </c>
+      <c r="D5" s="41">
+        <v>0.95</v>
+      </c>
+      <c r="E5" s="41">
+        <v>40</v>
+      </c>
+      <c r="F5" s="41">
+        <v>20</v>
+      </c>
+      <c r="G5" s="41">
+        <v>4</v>
+      </c>
+      <c r="H5" t="s" s="44">
+        <v>32</v>
+      </c>
+      <c r="I5" s="45">
+        <v>1.9</v>
+      </c>
+      <c r="J5" s="46">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="9">
-        <v>7</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="E2" t="s" s="9">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s" s="10">
+    </row>
+    <row r="6" ht="20.2" customHeight="1">
+      <c r="A6" t="s" s="39">
+        <v>33</v>
+      </c>
+      <c r="B6" s="40">
+        <v>20</v>
+      </c>
+      <c r="C6" s="41">
+        <v>1550</v>
+      </c>
+      <c r="D6" s="41">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="41">
+        <v>40</v>
+      </c>
+      <c r="F6" s="41">
+        <v>20</v>
+      </c>
+      <c r="G6" s="41">
+        <v>1</v>
+      </c>
+      <c r="H6" t="s" s="47">
+        <v>34</v>
+      </c>
+      <c r="I6" s="41">
+        <v>10.7</v>
+      </c>
+      <c r="J6" s="46">
+        <f>B6/2.2</f>
+        <v>9.09090909090909</v>
+      </c>
+    </row>
+    <row r="7" ht="20.2" customHeight="1">
+      <c r="A7" t="s" s="39">
+        <v>35</v>
+      </c>
+      <c r="B7" s="40">
+        <v>4</v>
+      </c>
+      <c r="C7" s="41">
+        <v>940</v>
+      </c>
+      <c r="D7" s="41">
+        <v>0.95</v>
+      </c>
+      <c r="E7" s="41">
+        <v>40</v>
+      </c>
+      <c r="F7" s="46">
+        <v>20</v>
+      </c>
+      <c r="G7" s="45">
+        <v>1</v>
+      </c>
+      <c r="H7" t="s" s="44">
+        <v>36</v>
+      </c>
+      <c r="I7" s="45">
+        <v>2</v>
+      </c>
+      <c r="J7" s="46">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" ht="20.2" customHeight="1">
+      <c r="A8" t="s" s="39">
+        <v>37</v>
+      </c>
+      <c r="B8" s="40">
+        <v>28</v>
+      </c>
+      <c r="C8" s="48">
+        <v>1375</v>
+      </c>
+      <c r="D8" s="41">
+        <v>0.95</v>
+      </c>
+      <c r="E8" s="41">
+        <v>40</v>
+      </c>
+      <c r="F8" s="41">
+        <v>20</v>
+      </c>
+      <c r="G8" s="41">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s" s="44">
+        <v>34</v>
+      </c>
+      <c r="I8" s="45">
+        <v>11.5</v>
+      </c>
+      <c r="J8" s="46">
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="9" ht="20.2" customHeight="1">
+      <c r="A9" t="s" s="39">
+        <v>38</v>
+      </c>
+      <c r="B9" s="40">
+        <f>50*0.5</f>
+        <v>25</v>
+      </c>
+      <c r="C9" s="36">
+        <v>850</v>
+      </c>
+      <c r="D9" s="41">
+        <v>0.95</v>
+      </c>
+      <c r="E9" s="41">
+        <v>70</v>
+      </c>
+      <c r="F9" s="41">
+        <v>60</v>
+      </c>
+      <c r="G9" s="41">
+        <v>2</v>
+      </c>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="43"/>
+    </row>
+    <row r="10" ht="20.2" customHeight="1">
+      <c r="A10" t="s" s="49">
+        <v>39</v>
+      </c>
+      <c r="B10" s="40">
+        <f>50*0.38</f>
+        <v>19</v>
+      </c>
+      <c r="C10" s="41">
+        <v>940</v>
+      </c>
+      <c r="D10" s="41">
+        <v>0.95</v>
+      </c>
+      <c r="E10" s="41">
+        <v>70</v>
+      </c>
+      <c r="F10" s="41">
+        <v>60</v>
+      </c>
+      <c r="G10" s="41">
+        <v>2</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="43"/>
+    </row>
+    <row r="11" ht="20.2" customHeight="1">
+      <c r="A11" t="s" s="50">
+        <v>40</v>
+      </c>
+      <c r="B11" s="40">
+        <f>50*0.22</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="11">
-        <v>12</v>
-      </c>
-      <c r="B3" s="12">
-        <v>20</v>
-      </c>
-      <c r="C3" s="13">
-        <v>850</v>
-      </c>
-      <c r="D3" s="13">
+      <c r="C11" s="41">
+        <v>1375</v>
+      </c>
+      <c r="D11" s="41">
         <v>0.95</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E11" s="41">
+        <v>70</v>
+      </c>
+      <c r="F11" s="41">
         <v>60</v>
       </c>
-      <c r="F3" s="14">
+      <c r="G11" s="41">
+        <v>4</v>
+      </c>
+      <c r="H11" s="42"/>
+      <c r="I11" s="42"/>
+      <c r="J11" s="43"/>
+    </row>
+    <row r="12" ht="20.2" customHeight="1">
+      <c r="A12" t="s" s="51">
+        <v>41</v>
+      </c>
+      <c r="B12" s="52">
+        <f>50*0.19+C14</f>
+        <v>9.5</v>
+      </c>
+      <c r="C12" s="41">
+        <v>1550</v>
+      </c>
+      <c r="D12" s="53">
+        <v>0.95</v>
+      </c>
+      <c r="E12" s="53">
+        <v>70</v>
+      </c>
+      <c r="F12" s="53">
         <v>60</v>
       </c>
-    </row>
-    <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="15">
-        <v>13</v>
-      </c>
-      <c r="B4" s="16">
-        <v>10</v>
-      </c>
-      <c r="C4" s="17">
-        <v>940</v>
-      </c>
-      <c r="D4" s="17">
-        <v>0.95</v>
-      </c>
-      <c r="E4" s="17">
-        <v>60</v>
-      </c>
-      <c r="F4" s="18">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="22"/>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="23"/>
-      <c r="B9" s="24"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="26"/>
+      <c r="G12" s="53">
+        <v>4</v>
+      </c>
+      <c r="H12" s="54"/>
+      <c r="I12" s="54"/>
+      <c r="J12" s="55"/>
+    </row>
+    <row r="13" ht="14.7" customHeight="1">
+      <c r="A13" s="56"/>
+      <c r="B13" s="57"/>
+      <c r="C13" s="58"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="59"/>
+    </row>
+    <row r="14" ht="14.7" customHeight="1">
+      <c r="A14" s="60"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="61"/>
+      <c r="D14" s="61"/>
+      <c r="E14" s="61"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="61"/>
+      <c r="H14" s="61"/>
+      <c r="I14" s="61"/>
+      <c r="J14" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="C1:H1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="H5" r:id="rId1" location="" tooltip="" display="https://www.thorlabs.com/drawings/471c86010a0aa6dc-F53DE964-0AE3-E9AF-406B86F1AA7C426E/L1550G1-SpecSheet.pdf"/>
+    <hyperlink ref="H6" r:id="rId2" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
+    <hyperlink ref="H7" r:id="rId3" location="" tooltip="" display="https://www.ii-vi.com/wp-content/uploads/2019/07/940nm-Multi-Mode-High-Power-VCSEL-Array-web-2-1.pdf"/>
+    <hyperlink ref="H8" r:id="rId4" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
+  </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;KFEFFFE&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2011,120 +3120,142 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="27" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="27" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="63" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" t="s" s="64">
+        <v>42</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" ht="20.45" customHeight="1">
+      <c r="A2" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="32">
+        <v>43</v>
+      </c>
+      <c r="C2" t="s" s="32">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s" s="32">
+        <v>45</v>
+      </c>
+      <c r="E2" s="65"/>
+    </row>
+    <row r="3" ht="20.45" customHeight="1">
+      <c r="A3" t="s" s="34">
+        <v>46</v>
+      </c>
+      <c r="B3" s="35">
+        <v>3</v>
+      </c>
+      <c r="C3" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="D3" s="36">
+        <v>1000</v>
+      </c>
+      <c r="E3" s="38"/>
+    </row>
+    <row r="4" ht="20.2" customHeight="1">
+      <c r="A4" t="s" s="39">
+        <v>47</v>
+      </c>
+      <c r="B4" s="40">
+        <v>60</v>
+      </c>
+      <c r="C4" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="D4" s="41">
+        <v>30000</v>
+      </c>
+      <c r="E4" s="43"/>
+    </row>
+    <row r="5" ht="20.2" customHeight="1">
+      <c r="A5" t="s" s="39">
+        <v>48</v>
+      </c>
+      <c r="B5" s="40">
+        <v>200</v>
+      </c>
+      <c r="C5" s="41">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="41">
+        <v>1</v>
+      </c>
+      <c r="E5" s="43"/>
+    </row>
+    <row r="6" ht="20.2" customHeight="1">
+      <c r="A6" t="s" s="39">
+        <v>49</v>
+      </c>
+      <c r="B6" s="40">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-    </row>
-    <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="8">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="9">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s" s="9">
-        <v>17</v>
-      </c>
-      <c r="E2" s="28"/>
-    </row>
-    <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="11">
-        <v>18</v>
-      </c>
-      <c r="B3" s="12">
-        <v>3</v>
-      </c>
-      <c r="C3" s="13">
+      <c r="C6" s="41">
         <v>0.5</v>
       </c>
-      <c r="D3" s="13">
-        <v>1000</v>
-      </c>
-      <c r="E3" s="29"/>
-    </row>
-    <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="15">
-        <v>19</v>
-      </c>
-      <c r="B4" s="16">
-        <v>60</v>
-      </c>
-      <c r="C4" s="17">
+      <c r="D6" s="41">
+        <v>100000</v>
+      </c>
+      <c r="E6" s="43"/>
+    </row>
+    <row r="7" ht="20.2" customHeight="1">
+      <c r="A7" t="s" s="39">
+        <v>50</v>
+      </c>
+      <c r="B7" s="40">
+        <v>5</v>
+      </c>
+      <c r="C7" s="41">
         <v>0.5</v>
       </c>
-      <c r="D4" s="17">
-        <v>30000</v>
-      </c>
-      <c r="E4" s="22"/>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
-    </row>
-    <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
+      <c r="D7" s="41">
+        <v>0.01</v>
+      </c>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="43"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="43"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2133,7 +3264,7 @@
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;KFEFFFE&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2143,114 +3274,128 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:E11"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="30" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="30" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="70" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="70" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="A1" t="s" s="64">
+        <v>51</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="30"/>
     </row>
     <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="8">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="9">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>9</v>
-      </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="28"/>
+      <c r="A2" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="32">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s" s="32">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="32">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s" s="33">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="11">
-        <v>22</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="A3" t="s" s="34">
+        <v>55</v>
+      </c>
+      <c r="B3" s="35">
         <v>2</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="36">
         <v>0.9</v>
       </c>
-      <c r="D3" s="32"/>
-      <c r="E3" s="29"/>
+      <c r="D3" s="71">
+        <v>0.005</v>
+      </c>
+      <c r="E3" s="72">
+        <v>50</v>
+      </c>
     </row>
     <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="15">
-        <v>23</v>
-      </c>
-      <c r="B4" s="16">
+      <c r="A4" t="s" s="39">
+        <v>56</v>
+      </c>
+      <c r="B4" s="40">
         <v>2.4</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="41">
         <v>0.9</v>
       </c>
-      <c r="D4" s="21"/>
-      <c r="E4" s="22"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="22"/>
+      <c r="A5" t="s" s="39">
+        <v>57</v>
+      </c>
+      <c r="B5" s="40">
+        <v>1.4</v>
+      </c>
+      <c r="C5" s="41">
+        <v>0.9</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="46">
+        <v>50</v>
+      </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="22"/>
+      <c r="A6" s="66"/>
+      <c r="B6" s="67"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43"/>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="22"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="22"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="43"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="22"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="22"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="43"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="26"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2259,7 +3404,7 @@
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;KFEFFFE&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2269,169 +3414,358 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:G11"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="7" width="16.3516" style="33" customWidth="1"/>
-    <col min="8" max="16384" width="16.3516" style="33" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="73" customWidth="1"/>
+    <col min="2" max="13" width="10.125" style="73" customWidth="1"/>
+    <col min="14" max="16384" width="16.3516" style="73" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="7">
+      <c r="A1" s="26"/>
+      <c r="B1" t="s" s="28">
+        <v>58</v>
+      </c>
+      <c r="C1" s="29"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="27"/>
+      <c r="M1" s="74"/>
+    </row>
+    <row r="2" ht="26.7" customHeight="1">
+      <c r="A2" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="32">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s" s="32">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s" s="32">
+        <v>61</v>
+      </c>
+      <c r="E2" t="s" s="32">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s" s="32">
+        <v>63</v>
+      </c>
+      <c r="G2" t="s" s="32">
+        <v>64</v>
+      </c>
+      <c r="H2" t="s" s="32">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s" s="32">
+        <v>66</v>
+      </c>
+      <c r="J2" t="s" s="32">
+        <v>67</v>
+      </c>
+      <c r="K2" t="s" s="32">
+        <v>68</v>
+      </c>
+      <c r="L2" t="s" s="32">
+        <v>69</v>
+      </c>
+      <c r="M2" t="s" s="33">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="3" ht="20.45" customHeight="1">
+      <c r="A3" t="s" s="34">
+        <v>71</v>
+      </c>
+      <c r="B3" s="75">
+        <v>4.5e-06</v>
+      </c>
+      <c r="C3" s="36">
+        <v>850</v>
+      </c>
+      <c r="D3" t="s" s="76">
+        <v>72</v>
+      </c>
+      <c r="E3" s="36">
+        <v>10</v>
+      </c>
+      <c r="F3" s="37"/>
+      <c r="G3" s="36">
+        <v>0.7</v>
+      </c>
+      <c r="H3" s="36">
+        <v>640</v>
+      </c>
+      <c r="I3" s="36">
+        <v>480</v>
+      </c>
+      <c r="J3" s="36">
         <v>5</v>
       </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-    </row>
-    <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="8">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="9">
-        <v>25</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>26</v>
-      </c>
-      <c r="D2" t="s" s="9">
-        <v>27</v>
-      </c>
-      <c r="E2" t="s" s="9">
-        <v>28</v>
-      </c>
-      <c r="F2" t="s" s="9">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s" s="10">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="11">
-        <v>31</v>
-      </c>
-      <c r="B3" s="34">
+      <c r="K3" s="36">
+        <v>5000</v>
+      </c>
+      <c r="L3" s="37"/>
+      <c r="M3" t="b" s="72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="20.2" customHeight="1">
+      <c r="A4" t="s" s="77">
+        <v>73</v>
+      </c>
+      <c r="B4" s="78">
         <v>4.5e-06</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C4" s="48">
+        <v>550</v>
+      </c>
+      <c r="D4" t="s" s="79">
+        <v>72</v>
+      </c>
+      <c r="E4" s="48">
+        <v>10</v>
+      </c>
+      <c r="F4" s="80"/>
+      <c r="G4" s="48">
+        <v>0.7</v>
+      </c>
+      <c r="H4" s="48">
+        <v>640</v>
+      </c>
+      <c r="I4" s="48">
+        <v>480</v>
+      </c>
+      <c r="J4" s="48">
+        <v>5</v>
+      </c>
+      <c r="K4" s="48">
+        <v>5000</v>
+      </c>
+      <c r="L4" s="80"/>
+      <c r="M4" t="b" s="81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" ht="20.2" customHeight="1">
+      <c r="A5" t="s" s="34">
+        <v>74</v>
+      </c>
+      <c r="B5" s="82">
+        <v>7.5e-06</v>
+      </c>
+      <c r="C5" s="36">
         <v>850</v>
       </c>
-      <c r="D3" s="13">
-        <v>0.3</v>
-      </c>
-      <c r="E3" s="13">
-        <v>0.7</v>
-      </c>
-      <c r="F3" s="13">
+      <c r="D5" t="s" s="76">
+        <v>72</v>
+      </c>
+      <c r="E5" s="36">
+        <v>10</v>
+      </c>
+      <c r="F5" s="37"/>
+      <c r="G5" s="36">
+        <v>1</v>
+      </c>
+      <c r="H5" s="36">
         <v>640</v>
       </c>
-      <c r="G3" s="14">
+      <c r="I5" s="36">
         <v>480</v>
       </c>
-    </row>
-    <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="15">
-        <v>32</v>
-      </c>
-      <c r="B4" s="35">
-        <v>4.5e-06</v>
-      </c>
-      <c r="C4" s="17">
-        <v>550</v>
-      </c>
-      <c r="D4" s="17">
-        <v>0.7</v>
-      </c>
-      <c r="E4" s="17">
-        <v>0.7</v>
-      </c>
-      <c r="F4" s="17">
-        <v>640</v>
-      </c>
-      <c r="G4" s="18">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="21"/>
-      <c r="D5" s="21"/>
-      <c r="E5" s="21"/>
-      <c r="F5" s="21"/>
-      <c r="G5" s="22"/>
+      <c r="J5" s="36">
+        <v>5</v>
+      </c>
+      <c r="K5" s="36">
+        <v>5000</v>
+      </c>
+      <c r="L5" s="83">
+        <v>1e-14</v>
+      </c>
+      <c r="M5" t="b" s="72">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="22"/>
+      <c r="A6" t="s" s="39">
+        <v>75</v>
+      </c>
+      <c r="B6" s="84">
+        <v>7.5e-06</v>
+      </c>
+      <c r="C6" s="41">
+        <v>940</v>
+      </c>
+      <c r="D6" t="s" s="47">
+        <v>72</v>
+      </c>
+      <c r="E6" s="41">
+        <v>10</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="41">
+        <v>1</v>
+      </c>
+      <c r="H6" s="41">
+        <v>1280</v>
+      </c>
+      <c r="I6" s="46">
+        <v>960</v>
+      </c>
+      <c r="J6" s="45">
+        <v>5</v>
+      </c>
+      <c r="K6" s="41">
+        <v>5000</v>
+      </c>
+      <c r="L6" s="85">
+        <v>1e-14</v>
+      </c>
+      <c r="M6" t="b" s="46">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="22"/>
+      <c r="A7" t="s" s="39">
+        <v>76</v>
+      </c>
+      <c r="B7" s="84">
+        <v>7.5e-06</v>
+      </c>
+      <c r="C7" s="41">
+        <v>1375</v>
+      </c>
+      <c r="D7" t="s" s="47">
+        <v>77</v>
+      </c>
+      <c r="E7" s="41">
+        <v>1</v>
+      </c>
+      <c r="F7" s="42"/>
+      <c r="G7" s="41">
+        <v>1</v>
+      </c>
+      <c r="H7" s="41">
+        <v>1280</v>
+      </c>
+      <c r="I7" s="46">
+        <v>960</v>
+      </c>
+      <c r="J7" s="45">
+        <v>5</v>
+      </c>
+      <c r="K7" s="41">
+        <v>5000</v>
+      </c>
+      <c r="L7" s="85">
+        <v>1e-14</v>
+      </c>
+      <c r="M7" t="b" s="46">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="22"/>
+      <c r="A8" t="s" s="39">
+        <v>78</v>
+      </c>
+      <c r="B8" s="84">
+        <v>7.5e-06</v>
+      </c>
+      <c r="C8" s="41">
+        <v>1550</v>
+      </c>
+      <c r="D8" t="s" s="47">
+        <v>77</v>
+      </c>
+      <c r="E8" s="41">
+        <v>1</v>
+      </c>
+      <c r="F8" s="42"/>
+      <c r="G8" s="41">
+        <v>1</v>
+      </c>
+      <c r="H8" s="41">
+        <v>1280</v>
+      </c>
+      <c r="I8" s="41">
+        <v>960</v>
+      </c>
+      <c r="J8" s="41">
+        <v>5</v>
+      </c>
+      <c r="K8" s="41">
+        <v>5000</v>
+      </c>
+      <c r="L8" s="85">
+        <v>1e-14</v>
+      </c>
+      <c r="M8" t="b" s="46">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="22"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="22"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="42"/>
+      <c r="M10" s="43"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="54"/>
+      <c r="M11" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;KFEFFFE&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2441,244 +3775,256 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:L11"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="12" width="16.3516" style="36" customWidth="1"/>
-    <col min="13" max="16384" width="16.3516" style="36" customWidth="1"/>
+    <col min="1" max="1" width="13.0859" style="86" customWidth="1"/>
+    <col min="2" max="2" width="9.72656" style="86" customWidth="1"/>
+    <col min="3" max="3" width="10.5391" style="86" customWidth="1"/>
+    <col min="4" max="11" width="9.72656" style="86" customWidth="1"/>
+    <col min="12" max="12" width="9.23438" style="86" customWidth="1"/>
+    <col min="13" max="16384" width="16.3516" style="86" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7"/>
-      <c r="L1" s="7"/>
-    </row>
-    <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="8">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s" s="9">
-        <v>34</v>
-      </c>
-      <c r="C2" t="s" s="9">
-        <v>35</v>
-      </c>
-      <c r="D2" t="s" s="9">
-        <v>36</v>
-      </c>
-      <c r="E2" t="s" s="9">
-        <v>37</v>
-      </c>
-      <c r="F2" t="s" s="9">
-        <v>38</v>
-      </c>
-      <c r="G2" t="s" s="9">
-        <v>39</v>
-      </c>
-      <c r="H2" t="s" s="9">
-        <v>40</v>
-      </c>
-      <c r="I2" t="s" s="9">
-        <v>41</v>
-      </c>
-      <c r="J2" t="s" s="9">
-        <v>42</v>
-      </c>
-      <c r="K2" t="s" s="9">
-        <v>43</v>
-      </c>
-      <c r="L2" t="s" s="10">
-        <v>44</v>
+      <c r="A1" t="s" s="64">
+        <v>79</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="30"/>
+    </row>
+    <row r="2" ht="26.7" customHeight="1">
+      <c r="A2" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="32">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s" s="32">
+        <v>81</v>
+      </c>
+      <c r="D2" t="s" s="32">
+        <v>82</v>
+      </c>
+      <c r="E2" t="s" s="32">
+        <v>83</v>
+      </c>
+      <c r="F2" t="s" s="32">
+        <v>84</v>
+      </c>
+      <c r="G2" t="s" s="32">
+        <v>85</v>
+      </c>
+      <c r="H2" t="s" s="32">
+        <v>86</v>
+      </c>
+      <c r="I2" t="s" s="32">
+        <v>87</v>
+      </c>
+      <c r="J2" t="s" s="32">
+        <v>88</v>
+      </c>
+      <c r="K2" t="s" s="32">
+        <v>89</v>
+      </c>
+      <c r="L2" t="s" s="33">
+        <v>90</v>
       </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="11">
-        <v>45</v>
-      </c>
-      <c r="B3" s="12">
+      <c r="A3" t="s" s="34">
+        <v>91</v>
+      </c>
+      <c r="B3" s="35">
         <v>30</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="36">
         <v>1</v>
       </c>
-      <c r="D3" s="13">
+      <c r="D3" s="36">
         <v>0.0036</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="36">
         <f>1/B3/2</f>
         <v>0.0166666666666667</v>
       </c>
-      <c r="F3" s="32"/>
-      <c r="G3" s="32"/>
-      <c r="H3" s="32"/>
-      <c r="I3" s="32"/>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
-      <c r="L3" s="29"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="38"/>
     </row>
     <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="15">
-        <v>46</v>
-      </c>
-      <c r="B4" s="16">
+      <c r="A4" t="s" s="39">
+        <v>92</v>
+      </c>
+      <c r="B4" s="40">
         <v>60</v>
       </c>
-      <c r="C4" s="17">
+      <c r="C4" s="41">
         <v>1</v>
       </c>
-      <c r="D4" s="17">
+      <c r="D4" s="41">
         <v>0.5</v>
       </c>
-      <c r="E4" s="17">
+      <c r="E4" s="41">
         <f>1/B4/2</f>
         <v>0.00833333333333333</v>
       </c>
-      <c r="F4" s="21"/>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="21"/>
-      <c r="J4" s="21"/>
-      <c r="K4" s="21"/>
-      <c r="L4" s="22"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="43"/>
     </row>
     <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="15">
-        <v>47</v>
-      </c>
-      <c r="B5" s="16">
+      <c r="A5" t="s" s="39">
+        <v>93</v>
+      </c>
+      <c r="B5" s="40">
         <v>30</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="41">
         <v>1000</v>
       </c>
-      <c r="D5" s="17">
+      <c r="D5" s="41">
         <v>0.0036</v>
       </c>
-      <c r="E5" s="17">
+      <c r="E5" s="41">
         <f>1/B5/10</f>
         <v>0.00333333333333333</v>
       </c>
-      <c r="F5" s="37">
+      <c r="F5" s="87">
         <v>3e-09</v>
       </c>
-      <c r="G5" s="37">
+      <c r="G5" s="87">
         <v>5e-09</v>
       </c>
-      <c r="H5" s="38">
+      <c r="H5" s="88">
         <v>1e-08</v>
       </c>
-      <c r="I5" s="37">
+      <c r="I5" s="87">
         <v>1e-09</v>
       </c>
-      <c r="J5" s="37">
+      <c r="J5" s="87">
         <v>1e-09</v>
       </c>
-      <c r="K5" s="38">
+      <c r="K5" s="88">
         <v>1e-08</v>
       </c>
-      <c r="L5" s="39">
+      <c r="L5" s="89">
         <v>3e-09</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="21"/>
-      <c r="G6" s="21"/>
-      <c r="H6" s="21"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="21"/>
-      <c r="K6" s="21"/>
-      <c r="L6" s="22"/>
+      <c r="A6" t="s" s="39">
+        <v>94</v>
+      </c>
+      <c r="B6" s="40">
+        <v>30</v>
+      </c>
+      <c r="C6" s="41">
+        <v>1</v>
+      </c>
+      <c r="D6" s="41">
+        <v>1</v>
+      </c>
+      <c r="E6" s="41">
+        <v>0.0001</v>
+      </c>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
+      <c r="H6" s="42"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="42"/>
+      <c r="K6" s="42"/>
+      <c r="L6" s="43"/>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="21"/>
-      <c r="G7" s="21"/>
-      <c r="H7" s="21"/>
-      <c r="I7" s="21"/>
-      <c r="J7" s="21"/>
-      <c r="K7" s="21"/>
-      <c r="L7" s="22"/>
+      <c r="A7" s="66"/>
+      <c r="B7" s="67"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="42"/>
+      <c r="F7" s="42"/>
+      <c r="G7" s="42"/>
+      <c r="H7" s="42"/>
+      <c r="I7" s="42"/>
+      <c r="J7" s="42"/>
+      <c r="K7" s="42"/>
+      <c r="L7" s="43"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="21"/>
-      <c r="G8" s="21"/>
-      <c r="H8" s="21"/>
-      <c r="I8" s="21"/>
-      <c r="J8" s="21"/>
-      <c r="K8" s="21"/>
-      <c r="L8" s="22"/>
+      <c r="A8" s="66"/>
+      <c r="B8" s="67"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="42"/>
+      <c r="F8" s="42"/>
+      <c r="G8" s="42"/>
+      <c r="H8" s="42"/>
+      <c r="I8" s="42"/>
+      <c r="J8" s="42"/>
+      <c r="K8" s="42"/>
+      <c r="L8" s="43"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="21"/>
-      <c r="G9" s="21"/>
-      <c r="H9" s="21"/>
-      <c r="I9" s="21"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="21"/>
-      <c r="L9" s="22"/>
+      <c r="A9" s="66"/>
+      <c r="B9" s="67"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="21"/>
-      <c r="G10" s="21"/>
-      <c r="H10" s="21"/>
-      <c r="I10" s="21"/>
-      <c r="J10" s="21"/>
-      <c r="K10" s="21"/>
-      <c r="L10" s="22"/>
+      <c r="A10" s="66"/>
+      <c r="B10" s="67"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="42"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="42"/>
+      <c r="H10" s="42"/>
+      <c r="I10" s="42"/>
+      <c r="J10" s="42"/>
+      <c r="K10" s="42"/>
+      <c r="L10" s="43"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="26"/>
+      <c r="A11" s="68"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="54"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
+      <c r="J11" s="54"/>
+      <c r="K11" s="54"/>
+      <c r="L11" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2687,7 +4033,7 @@
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;KFEFFFE&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
@@ -2697,155 +4043,265 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="B3" xSplit="1" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="40" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="40" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="90" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="90" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
+      <c r="A1" t="s" s="64">
+        <v>95</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="30"/>
     </row>
     <row r="2" ht="20.45" customHeight="1">
-      <c r="A2" t="s" s="8">
+      <c r="A2" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="32">
         <v>6</v>
       </c>
-      <c r="B2" t="s" s="9">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s" s="9">
+      <c r="C2" t="s" s="32">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s" s="32">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s" s="32">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s" s="33">
         <v>14</v>
       </c>
-      <c r="D2" t="s" s="9">
-        <v>20</v>
-      </c>
-      <c r="E2" t="s" s="9">
-        <v>24</v>
-      </c>
-      <c r="F2" t="s" s="10">
-        <v>33</v>
-      </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
-      <c r="A3" t="s" s="11">
+      <c r="A3" t="s" s="34">
+        <v>96</v>
+      </c>
+      <c r="B3" t="s" s="91">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s" s="92">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s" s="76">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s" s="92">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s" s="93">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="4" ht="20.2" customHeight="1">
+      <c r="A4" t="s" s="39">
+        <v>97</v>
+      </c>
+      <c r="B4" t="s" s="94">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s" s="95">
+        <v>98</v>
+      </c>
+      <c r="D4" t="s" s="47">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s" s="95">
+        <v>73</v>
+      </c>
+      <c r="F4" t="s" s="96">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="5" ht="20.2" customHeight="1">
+      <c r="A5" t="s" s="39">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s" s="94">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s" s="95">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s" s="47">
+        <v>55</v>
+      </c>
+      <c r="E5" t="s" s="95">
+        <v>71</v>
+      </c>
+      <c r="F5" t="s" s="96">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="6" ht="20.2" customHeight="1">
+      <c r="A6" t="s" s="97">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s" s="98">
+        <v>38</v>
+      </c>
+      <c r="C6" t="s" s="39">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s" s="94">
+        <v>57</v>
+      </c>
+      <c r="E6" t="s" s="99">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s" s="96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="7" ht="20.2" customHeight="1">
+      <c r="A7" t="s" s="39">
+        <v>101</v>
+      </c>
+      <c r="B7" t="s" s="100">
+        <v>39</v>
+      </c>
+      <c r="C7" t="s" s="39">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s" s="94">
+        <v>57</v>
+      </c>
+      <c r="E7" t="s" s="99">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s" s="96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="8" ht="20.2" customHeight="1">
+      <c r="A8" t="s" s="39">
+        <v>102</v>
+      </c>
+      <c r="B8" t="s" s="101">
+        <v>40</v>
+      </c>
+      <c r="C8" t="s" s="39">
+        <v>50</v>
+      </c>
+      <c r="D8" t="s" s="94">
+        <v>57</v>
+      </c>
+      <c r="E8" t="s" s="99">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s" s="96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="9" ht="20.2" customHeight="1">
+      <c r="A9" t="s" s="39">
+        <v>103</v>
+      </c>
+      <c r="B9" t="s" s="101">
+        <v>41</v>
+      </c>
+      <c r="C9" t="s" s="39">
+        <v>50</v>
+      </c>
+      <c r="D9" t="s" s="94">
+        <v>57</v>
+      </c>
+      <c r="E9" t="s" s="99">
+        <v>78</v>
+      </c>
+      <c r="F9" t="s" s="96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" ht="20.2" customHeight="1">
+      <c r="A10" t="s" s="97">
+        <v>104</v>
+      </c>
+      <c r="B10" t="s" s="98">
+        <v>38</v>
+      </c>
+      <c r="C10" t="s" s="39">
         <v>49</v>
       </c>
-      <c r="B3" t="s" s="41">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s" s="42">
-        <v>18</v>
-      </c>
-      <c r="D3" t="s" s="42">
-        <v>22</v>
-      </c>
-      <c r="E3" t="s" s="43">
-        <v>31</v>
-      </c>
-      <c r="F3" t="s" s="44">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="15">
-        <v>50</v>
-      </c>
-      <c r="B4" t="s" s="45">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s" s="46">
-        <v>18</v>
-      </c>
-      <c r="D4" t="s" s="46">
-        <v>23</v>
-      </c>
-      <c r="E4" t="s" s="47">
-        <v>32</v>
-      </c>
-      <c r="F4" t="s" s="48">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="15">
-        <v>51</v>
-      </c>
-      <c r="B5" t="s" s="45">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s" s="46">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s" s="46">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s" s="47">
-        <v>31</v>
-      </c>
-      <c r="F5" t="s" s="48">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="21"/>
-      <c r="D6" s="21"/>
-      <c r="E6" s="21"/>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
-      <c r="F7" s="22"/>
-    </row>
-    <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
-      <c r="D8" s="21"/>
-      <c r="E8" s="21"/>
-      <c r="F8" s="22"/>
-    </row>
-    <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21"/>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22"/>
-    </row>
-    <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="21"/>
-      <c r="E10" s="21"/>
-      <c r="F10" s="22"/>
+      <c r="D10" t="s" s="94">
+        <v>57</v>
+      </c>
+      <c r="E10" t="s" s="99">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s" s="96">
+        <v>94</v>
+      </c>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="23"/>
-      <c r="B11" s="24"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="26"/>
+      <c r="A11" t="s" s="39">
+        <v>105</v>
+      </c>
+      <c r="B11" t="s" s="100">
+        <v>39</v>
+      </c>
+      <c r="C11" t="s" s="39">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s" s="94">
+        <v>57</v>
+      </c>
+      <c r="E11" t="s" s="99">
+        <v>75</v>
+      </c>
+      <c r="F11" t="s" s="96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="12" ht="20.2" customHeight="1">
+      <c r="A12" t="s" s="39">
+        <v>106</v>
+      </c>
+      <c r="B12" t="s" s="101">
+        <v>40</v>
+      </c>
+      <c r="C12" t="s" s="39">
+        <v>49</v>
+      </c>
+      <c r="D12" t="s" s="94">
+        <v>57</v>
+      </c>
+      <c r="E12" t="s" s="99">
+        <v>76</v>
+      </c>
+      <c r="F12" t="s" s="96">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" ht="20.2" customHeight="1">
+      <c r="A13" t="s" s="39">
+        <v>107</v>
+      </c>
+      <c r="B13" t="s" s="101">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s" s="39">
+        <v>49</v>
+      </c>
+      <c r="D13" t="s" s="94">
+        <v>57</v>
+      </c>
+      <c r="E13" t="s" s="99">
+        <v>78</v>
+      </c>
+      <c r="F13" t="s" s="96">
+        <v>94</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2854,7 +4310,7 @@
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;KFEFFFE&amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add  overide configs' values
</commit_message>
<xml_diff>
--- a/data/photonic_simul_data.xlsx
+++ b/data/photonic_simul_data.xlsx
@@ -145,13 +145,13 @@
     <t>Number_units</t>
   </si>
   <si>
+    <t>Voltage_V</t>
+  </si>
+  <si>
+    <t>Current_A</t>
+  </si>
+  <si>
     <t>Link</t>
-  </si>
-  <si>
-    <t>Voltage_V</t>
-  </si>
-  <si>
-    <t>Current_A</t>
   </si>
   <si>
     <t>Laser1</t>
@@ -268,7 +268,7 @@
     <t xml:space="preserve">Sensor Table </t>
   </si>
   <si>
-    <t>PixelSize_m</t>
+    <t>PixSz_um</t>
   </si>
   <si>
     <t>Wavelength</t>
@@ -286,19 +286,19 @@
     <t>FF</t>
   </si>
   <si>
-    <t>ArrayRes_H</t>
-  </si>
-  <si>
-    <t>ArrayRes_V</t>
-  </si>
-  <si>
-    <t>ReadoutNoise_e</t>
-  </si>
-  <si>
-    <t>DarkSignal_e_s</t>
-  </si>
-  <si>
-    <t>Cfd_farad</t>
+    <t>Res_H</t>
+  </si>
+  <si>
+    <t>Res_V</t>
+  </si>
+  <si>
+    <t>RdNoise_e</t>
+  </si>
+  <si>
+    <t>DkSig_e_s</t>
+  </si>
+  <si>
+    <t>Cfd_fF</t>
   </si>
   <si>
     <t>CDS</t>
@@ -419,14 +419,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="5">
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="0.0##E+00"/>
     <numFmt numFmtId="60" formatCode="0.0?#####E+00"/>
-    <numFmt numFmtId="61" formatCode="0.0######E+00"/>
-    <numFmt numFmtId="62" formatCode="0.0#############E+00"/>
-    <numFmt numFmtId="63" formatCode="0.0?#######E+00"/>
-    <numFmt numFmtId="64" formatCode="0.0?######E+00"/>
+    <numFmt numFmtId="61" formatCode="0.0?#######E+00"/>
+    <numFmt numFmtId="62" formatCode="0.0?######E+00"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1081,7 +1079,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1166,12 +1164,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="6" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1217,13 +1215,10 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1328,28 +1323,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="61" fontId="0" fillId="6" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="62" fontId="0" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="61" fontId="0" fillId="6" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="62" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="63" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="64" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="63" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="61" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2741,15 +2727,15 @@
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" s="26"/>
       <c r="B1" s="27"/>
-      <c r="C1" t="s" s="28">
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" t="s" s="29">
         <v>18</v>
       </c>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
       <c r="J1" s="30"/>
     </row>
     <row r="2" ht="26.7" customHeight="1">
@@ -2858,14 +2844,14 @@
       <c r="G5" s="41">
         <v>4</v>
       </c>
-      <c r="H5" t="s" s="44">
+      <c r="H5" s="41">
+        <v>1.9</v>
+      </c>
+      <c r="I5" s="41">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s" s="44">
         <v>32</v>
-      </c>
-      <c r="I5" s="45">
-        <v>1.9</v>
-      </c>
-      <c r="J5" s="46">
-        <v>6</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
@@ -2890,15 +2876,15 @@
       <c r="G6" s="41">
         <v>1</v>
       </c>
-      <c r="H6" t="s" s="47">
-        <v>34</v>
+      <c r="H6" s="41">
+        <v>10.7</v>
       </c>
       <c r="I6" s="41">
-        <v>10.7</v>
-      </c>
-      <c r="J6" s="46">
         <f>B6/2.2</f>
         <v>9.09090909090909</v>
+      </c>
+      <c r="J6" t="s" s="44">
+        <v>34</v>
       </c>
     </row>
     <row r="7" ht="20.2" customHeight="1">
@@ -2917,20 +2903,20 @@
       <c r="E7" s="41">
         <v>40</v>
       </c>
-      <c r="F7" s="46">
+      <c r="F7" s="45">
         <v>20</v>
       </c>
-      <c r="G7" s="45">
+      <c r="G7" s="46">
         <v>1</v>
       </c>
-      <c r="H7" t="s" s="44">
+      <c r="H7" s="41">
+        <v>2</v>
+      </c>
+      <c r="I7" s="41">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s" s="44">
         <v>36</v>
-      </c>
-      <c r="I7" s="45">
-        <v>2</v>
-      </c>
-      <c r="J7" s="46">
-        <v>6</v>
       </c>
     </row>
     <row r="8" ht="20.2" customHeight="1">
@@ -2940,7 +2926,7 @@
       <c r="B8" s="40">
         <v>28</v>
       </c>
-      <c r="C8" s="48">
+      <c r="C8" s="47">
         <v>1375</v>
       </c>
       <c r="D8" s="41">
@@ -2955,14 +2941,14 @@
       <c r="G8" s="41">
         <v>1</v>
       </c>
-      <c r="H8" t="s" s="44">
+      <c r="H8" s="41">
+        <v>11.5</v>
+      </c>
+      <c r="I8" s="41">
+        <v>12.5</v>
+      </c>
+      <c r="J8" t="s" s="44">
         <v>34</v>
-      </c>
-      <c r="I8" s="45">
-        <v>11.5</v>
-      </c>
-      <c r="J8" s="46">
-        <v>12.5</v>
       </c>
     </row>
     <row r="9" ht="20.2" customHeight="1">
@@ -2993,7 +2979,7 @@
       <c r="J9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" t="s" s="49">
+      <c r="A10" t="s" s="48">
         <v>39</v>
       </c>
       <c r="B10" s="40">
@@ -3020,7 +3006,7 @@
       <c r="J10" s="43"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" t="s" s="50">
+      <c r="A11" t="s" s="49">
         <v>40</v>
       </c>
       <c r="B11" s="40">
@@ -3040,72 +3026,69 @@
         <v>60</v>
       </c>
       <c r="G11" s="41">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="H11" s="42"/>
       <c r="I11" s="42"/>
       <c r="J11" s="43"/>
     </row>
     <row r="12" ht="20.2" customHeight="1">
-      <c r="A12" t="s" s="51">
+      <c r="A12" t="s" s="50">
         <v>41</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B12" s="51">
         <f>50*0.19+C14</f>
         <v>9.5</v>
       </c>
       <c r="C12" s="41">
         <v>1550</v>
       </c>
-      <c r="D12" s="53">
+      <c r="D12" s="52">
         <v>0.95</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="52">
         <v>70</v>
       </c>
-      <c r="F12" s="53">
+      <c r="F12" s="52">
         <v>60</v>
       </c>
-      <c r="G12" s="53">
-        <v>4</v>
-      </c>
-      <c r="H12" s="54"/>
-      <c r="I12" s="54"/>
-      <c r="J12" s="55"/>
+      <c r="G12" s="52">
+        <v>2</v>
+      </c>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="54"/>
     </row>
     <row r="13" ht="14.7" customHeight="1">
-      <c r="A13" s="56"/>
-      <c r="B13" s="57"/>
-      <c r="C13" s="58"/>
-      <c r="D13" s="57"/>
-      <c r="E13" s="57"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="57"/>
-      <c r="H13" s="57"/>
-      <c r="I13" s="57"/>
-      <c r="J13" s="59"/>
+      <c r="A13" s="55"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="57"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
+      <c r="G13" s="56"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="56"/>
+      <c r="J13" s="58"/>
     </row>
     <row r="14" ht="14.7" customHeight="1">
-      <c r="A14" s="60"/>
-      <c r="B14" s="61"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="61"/>
-      <c r="F14" s="61"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="61"/>
-      <c r="J14" s="62"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C1:H1"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H5" r:id="rId1" location="" tooltip="" display="https://www.thorlabs.com/drawings/471c86010a0aa6dc-F53DE964-0AE3-E9AF-406B86F1AA7C426E/L1550G1-SpecSheet.pdf"/>
-    <hyperlink ref="H6" r:id="rId2" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
-    <hyperlink ref="H7" r:id="rId3" location="" tooltip="" display="https://www.ii-vi.com/wp-content/uploads/2019/07/940nm-Multi-Mode-High-Power-VCSEL-Array-web-2-1.pdf"/>
-    <hyperlink ref="H8" r:id="rId4" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
+    <hyperlink ref="J5" r:id="rId1" location="" tooltip="" display="https://www.thorlabs.com/drawings/471c86010a0aa6dc-F53DE964-0AE3-E9AF-406B86F1AA7C426E/L1550G1-SpecSheet.pdf"/>
+    <hyperlink ref="J6" r:id="rId2" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
+    <hyperlink ref="J7" r:id="rId3" location="" tooltip="" display="https://www.ii-vi.com/wp-content/uploads/2019/07/940nm-Multi-Mode-High-Power-VCSEL-Array-web-2-1.pdf"/>
+    <hyperlink ref="J8" r:id="rId4" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -3126,17 +3109,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="63" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="63" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="62" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="62" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="64">
+      <c r="A1" t="s" s="63">
         <v>42</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="30"/>
     </row>
     <row r="2" ht="20.45" customHeight="1">
@@ -3152,7 +3135,7 @@
       <c r="D2" t="s" s="32">
         <v>45</v>
       </c>
-      <c r="E2" s="65"/>
+      <c r="E2" s="64"/>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
@@ -3230,32 +3213,32 @@
       <c r="E7" s="43"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="66"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
       <c r="E8" s="43"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="66"/>
-      <c r="B9" s="67"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
       <c r="E9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
       <c r="E10" s="43"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="68"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3280,17 +3263,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="70" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="70" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="69" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="69" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="64">
+      <c r="A1" t="s" s="63">
         <v>51</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
       <c r="E1" s="30"/>
     </row>
     <row r="2" ht="20.45" customHeight="1">
@@ -3320,10 +3303,10 @@
       <c r="C3" s="36">
         <v>0.9</v>
       </c>
-      <c r="D3" s="71">
+      <c r="D3" s="70">
         <v>0.005</v>
       </c>
-      <c r="E3" s="72">
+      <c r="E3" s="71">
         <v>50</v>
       </c>
     </row>
@@ -3351,51 +3334,51 @@
         <v>0.9</v>
       </c>
       <c r="D5" s="42"/>
-      <c r="E5" s="46">
+      <c r="E5" s="45">
         <v>50</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" s="66"/>
-      <c r="B6" s="67"/>
+      <c r="A6" s="65"/>
+      <c r="B6" s="66"/>
       <c r="C6" s="42"/>
       <c r="D6" s="42"/>
       <c r="E6" s="43"/>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="66"/>
-      <c r="B7" s="67"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
       <c r="E7" s="43"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="66"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
       <c r="E8" s="43"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="66"/>
-      <c r="B9" s="67"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
       <c r="E9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
       <c r="E10" s="43"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="68"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="55"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3420,27 +3403,27 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="73" customWidth="1"/>
-    <col min="2" max="13" width="10.125" style="73" customWidth="1"/>
-    <col min="14" max="16384" width="16.3516" style="73" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="72" customWidth="1"/>
+    <col min="2" max="13" width="10.125" style="72" customWidth="1"/>
+    <col min="14" max="16384" width="16.3516" style="72" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" s="26"/>
-      <c r="B1" t="s" s="28">
+      <c r="B1" t="s" s="29">
         <v>58</v>
       </c>
-      <c r="C1" s="29"/>
+      <c r="C1" s="28"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
       <c r="K1" s="27"/>
       <c r="L1" s="27"/>
-      <c r="M1" s="74"/>
+      <c r="M1" s="73"/>
     </row>
     <row r="2" ht="26.7" customHeight="1">
       <c r="A2" t="s" s="31">
@@ -3487,13 +3470,13 @@
       <c r="A3" t="s" s="34">
         <v>71</v>
       </c>
-      <c r="B3" s="75">
-        <v>4.5e-06</v>
+      <c r="B3" s="74">
+        <v>3</v>
       </c>
       <c r="C3" s="36">
         <v>850</v>
       </c>
-      <c r="D3" t="s" s="76">
+      <c r="D3" t="s" s="75">
         <v>72</v>
       </c>
       <c r="E3" s="36">
@@ -3516,44 +3499,44 @@
         <v>5000</v>
       </c>
       <c r="L3" s="37"/>
-      <c r="M3" t="b" s="72">
+      <c r="M3" t="b" s="71">
         <v>1</v>
       </c>
     </row>
     <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="77">
+      <c r="A4" t="s" s="76">
         <v>73</v>
       </c>
-      <c r="B4" s="78">
-        <v>4.5e-06</v>
-      </c>
-      <c r="C4" s="48">
+      <c r="B4" s="77">
+        <v>3</v>
+      </c>
+      <c r="C4" s="47">
         <v>550</v>
       </c>
-      <c r="D4" t="s" s="79">
+      <c r="D4" t="s" s="78">
         <v>72</v>
       </c>
-      <c r="E4" s="48">
+      <c r="E4" s="47">
         <v>10</v>
       </c>
-      <c r="F4" s="80"/>
-      <c r="G4" s="48">
+      <c r="F4" s="79"/>
+      <c r="G4" s="47">
         <v>0.7</v>
       </c>
-      <c r="H4" s="48">
+      <c r="H4" s="47">
         <v>640</v>
       </c>
-      <c r="I4" s="48">
+      <c r="I4" s="47">
         <v>480</v>
       </c>
-      <c r="J4" s="48">
+      <c r="J4" s="47">
         <v>5</v>
       </c>
-      <c r="K4" s="48">
+      <c r="K4" s="47">
         <v>5000</v>
       </c>
-      <c r="L4" s="80"/>
-      <c r="M4" t="b" s="81">
+      <c r="L4" s="79"/>
+      <c r="M4" t="b" s="80">
         <v>1</v>
       </c>
     </row>
@@ -3561,13 +3544,13 @@
       <c r="A5" t="s" s="34">
         <v>74</v>
       </c>
-      <c r="B5" s="82">
-        <v>7.5e-06</v>
+      <c r="B5" s="35">
+        <v>7.5</v>
       </c>
       <c r="C5" s="36">
         <v>850</v>
       </c>
-      <c r="D5" t="s" s="76">
+      <c r="D5" t="s" s="75">
         <v>72</v>
       </c>
       <c r="E5" s="36">
@@ -3589,10 +3572,10 @@
       <c r="K5" s="36">
         <v>5000</v>
       </c>
-      <c r="L5" s="83">
-        <v>1e-14</v>
-      </c>
-      <c r="M5" t="b" s="72">
+      <c r="L5" s="36">
+        <v>10</v>
+      </c>
+      <c r="M5" t="b" s="71">
         <v>0</v>
       </c>
     </row>
@@ -3600,13 +3583,13 @@
       <c r="A6" t="s" s="39">
         <v>75</v>
       </c>
-      <c r="B6" s="84">
-        <v>7.5e-06</v>
+      <c r="B6" s="40">
+        <v>7.5</v>
       </c>
       <c r="C6" s="41">
         <v>940</v>
       </c>
-      <c r="D6" t="s" s="47">
+      <c r="D6" t="s" s="81">
         <v>72</v>
       </c>
       <c r="E6" s="41">
@@ -3617,21 +3600,21 @@
         <v>1</v>
       </c>
       <c r="H6" s="41">
-        <v>1280</v>
-      </c>
-      <c r="I6" s="46">
-        <v>960</v>
-      </c>
-      <c r="J6" s="45">
+        <v>640</v>
+      </c>
+      <c r="I6" s="45">
+        <v>480</v>
+      </c>
+      <c r="J6" s="46">
         <v>5</v>
       </c>
       <c r="K6" s="41">
         <v>5000</v>
       </c>
-      <c r="L6" s="85">
-        <v>1e-14</v>
-      </c>
-      <c r="M6" t="b" s="46">
+      <c r="L6" s="41">
+        <v>10</v>
+      </c>
+      <c r="M6" t="b" s="45">
         <v>0</v>
       </c>
     </row>
@@ -3639,13 +3622,13 @@
       <c r="A7" t="s" s="39">
         <v>76</v>
       </c>
-      <c r="B7" s="84">
-        <v>7.5e-06</v>
+      <c r="B7" s="40">
+        <v>7.5</v>
       </c>
       <c r="C7" s="41">
         <v>1375</v>
       </c>
-      <c r="D7" t="s" s="47">
+      <c r="D7" t="s" s="81">
         <v>77</v>
       </c>
       <c r="E7" s="41">
@@ -3656,21 +3639,21 @@
         <v>1</v>
       </c>
       <c r="H7" s="41">
-        <v>1280</v>
-      </c>
-      <c r="I7" s="46">
-        <v>960</v>
-      </c>
-      <c r="J7" s="45">
+        <v>640</v>
+      </c>
+      <c r="I7" s="45">
+        <v>480</v>
+      </c>
+      <c r="J7" s="46">
         <v>5</v>
       </c>
       <c r="K7" s="41">
         <v>5000</v>
       </c>
-      <c r="L7" s="85">
-        <v>1e-14</v>
-      </c>
-      <c r="M7" t="b" s="46">
+      <c r="L7" s="41">
+        <v>10</v>
+      </c>
+      <c r="M7" t="b" s="45">
         <v>0</v>
       </c>
     </row>
@@ -3678,13 +3661,13 @@
       <c r="A8" t="s" s="39">
         <v>78</v>
       </c>
-      <c r="B8" s="84">
-        <v>7.5e-06</v>
+      <c r="B8" s="40">
+        <v>7.5</v>
       </c>
       <c r="C8" s="41">
         <v>1550</v>
       </c>
-      <c r="D8" t="s" s="47">
+      <c r="D8" t="s" s="81">
         <v>77</v>
       </c>
       <c r="E8" s="41">
@@ -3695,10 +3678,10 @@
         <v>1</v>
       </c>
       <c r="H8" s="41">
-        <v>1280</v>
+        <v>640</v>
       </c>
       <c r="I8" s="41">
-        <v>960</v>
+        <v>480</v>
       </c>
       <c r="J8" s="41">
         <v>5</v>
@@ -3706,16 +3689,16 @@
       <c r="K8" s="41">
         <v>5000</v>
       </c>
-      <c r="L8" s="85">
-        <v>1e-14</v>
-      </c>
-      <c r="M8" t="b" s="46">
+      <c r="L8" s="41">
+        <v>10</v>
+      </c>
+      <c r="M8" t="b" s="45">
         <v>0</v>
       </c>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="66"/>
-      <c r="B9" s="67"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
       <c r="E9" s="42"/>
@@ -3729,8 +3712,8 @@
       <c r="M9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
@@ -3744,19 +3727,19 @@
       <c r="M10" s="43"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="68"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="54"/>
-      <c r="M11" s="55"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="53"/>
+      <c r="M11" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3781,28 +3764,28 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.0859" style="86" customWidth="1"/>
-    <col min="2" max="2" width="9.72656" style="86" customWidth="1"/>
-    <col min="3" max="3" width="10.5391" style="86" customWidth="1"/>
-    <col min="4" max="11" width="9.72656" style="86" customWidth="1"/>
-    <col min="12" max="12" width="9.23438" style="86" customWidth="1"/>
-    <col min="13" max="16384" width="16.3516" style="86" customWidth="1"/>
+    <col min="1" max="1" width="13.0859" style="82" customWidth="1"/>
+    <col min="2" max="2" width="9.72656" style="82" customWidth="1"/>
+    <col min="3" max="3" width="10.5391" style="82" customWidth="1"/>
+    <col min="4" max="11" width="9.72656" style="82" customWidth="1"/>
+    <col min="12" max="12" width="9.23438" style="82" customWidth="1"/>
+    <col min="13" max="16384" width="16.3516" style="82" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="64">
+      <c r="A1" t="s" s="63">
         <v>79</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
       <c r="L1" s="30"/>
     </row>
     <row r="2" ht="26.7" customHeight="1">
@@ -3910,25 +3893,25 @@
         <f>1/B5/10</f>
         <v>0.00333333333333333</v>
       </c>
-      <c r="F5" s="87">
+      <c r="F5" s="83">
         <v>3e-09</v>
       </c>
-      <c r="G5" s="87">
+      <c r="G5" s="83">
         <v>5e-09</v>
       </c>
-      <c r="H5" s="88">
+      <c r="H5" s="84">
         <v>1e-08</v>
       </c>
-      <c r="I5" s="87">
+      <c r="I5" s="83">
         <v>1e-09</v>
       </c>
-      <c r="J5" s="87">
+      <c r="J5" s="83">
         <v>1e-09</v>
       </c>
-      <c r="K5" s="88">
+      <c r="K5" s="84">
         <v>1e-08</v>
       </c>
-      <c r="L5" s="89">
+      <c r="L5" s="85">
         <v>3e-09</v>
       </c>
     </row>
@@ -3957,8 +3940,8 @@
       <c r="L6" s="43"/>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="66"/>
-      <c r="B7" s="67"/>
+      <c r="A7" s="65"/>
+      <c r="B7" s="66"/>
       <c r="C7" s="42"/>
       <c r="D7" s="42"/>
       <c r="E7" s="42"/>
@@ -3971,8 +3954,8 @@
       <c r="L7" s="43"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="66"/>
-      <c r="B8" s="67"/>
+      <c r="A8" s="65"/>
+      <c r="B8" s="66"/>
       <c r="C8" s="42"/>
       <c r="D8" s="42"/>
       <c r="E8" s="42"/>
@@ -3985,8 +3968,8 @@
       <c r="L8" s="43"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="66"/>
-      <c r="B9" s="67"/>
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
       <c r="C9" s="42"/>
       <c r="D9" s="42"/>
       <c r="E9" s="42"/>
@@ -3999,8 +3982,8 @@
       <c r="L9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="66"/>
-      <c r="B10" s="67"/>
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
       <c r="E10" s="42"/>
@@ -4013,18 +3996,18 @@
       <c r="L10" s="43"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="68"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="54"/>
-      <c r="D11" s="54"/>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
-      <c r="J11" s="54"/>
-      <c r="K11" s="54"/>
-      <c r="L11" s="55"/>
+      <c r="A11" s="67"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="53"/>
+      <c r="J11" s="53"/>
+      <c r="K11" s="53"/>
+      <c r="L11" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4049,18 +4032,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="90" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="90" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="86" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="86" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="64">
+      <c r="A1" t="s" s="63">
         <v>95</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="30"/>
     </row>
     <row r="2" ht="20.45" customHeight="1">
@@ -4087,19 +4070,19 @@
       <c r="A3" t="s" s="34">
         <v>96</v>
       </c>
-      <c r="B3" t="s" s="91">
+      <c r="B3" t="s" s="87">
         <v>29</v>
       </c>
-      <c r="C3" t="s" s="92">
+      <c r="C3" t="s" s="88">
         <v>46</v>
       </c>
-      <c r="D3" t="s" s="76">
+      <c r="D3" t="s" s="75">
         <v>55</v>
       </c>
-      <c r="E3" t="s" s="92">
+      <c r="E3" t="s" s="88">
         <v>71</v>
       </c>
-      <c r="F3" t="s" s="93">
+      <c r="F3" t="s" s="89">
         <v>91</v>
       </c>
     </row>
@@ -4107,19 +4090,19 @@
       <c r="A4" t="s" s="39">
         <v>97</v>
       </c>
-      <c r="B4" t="s" s="94">
+      <c r="B4" t="s" s="90">
         <v>30</v>
       </c>
-      <c r="C4" t="s" s="95">
+      <c r="C4" t="s" s="91">
         <v>98</v>
       </c>
-      <c r="D4" t="s" s="47">
+      <c r="D4" t="s" s="81">
         <v>56</v>
       </c>
-      <c r="E4" t="s" s="95">
+      <c r="E4" t="s" s="91">
         <v>73</v>
       </c>
-      <c r="F4" t="s" s="96">
+      <c r="F4" t="s" s="92">
         <v>92</v>
       </c>
     </row>
@@ -4127,39 +4110,39 @@
       <c r="A5" t="s" s="39">
         <v>99</v>
       </c>
-      <c r="B5" t="s" s="94">
+      <c r="B5" t="s" s="90">
         <v>29</v>
       </c>
-      <c r="C5" t="s" s="95">
+      <c r="C5" t="s" s="91">
         <v>48</v>
       </c>
-      <c r="D5" t="s" s="47">
+      <c r="D5" t="s" s="81">
         <v>55</v>
       </c>
-      <c r="E5" t="s" s="95">
+      <c r="E5" t="s" s="91">
         <v>71</v>
       </c>
-      <c r="F5" t="s" s="96">
+      <c r="F5" t="s" s="92">
         <v>93</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="97">
+      <c r="A6" t="s" s="93">
         <v>100</v>
       </c>
-      <c r="B6" t="s" s="98">
+      <c r="B6" t="s" s="94">
         <v>38</v>
       </c>
       <c r="C6" t="s" s="39">
         <v>50</v>
       </c>
-      <c r="D6" t="s" s="94">
+      <c r="D6" t="s" s="90">
         <v>57</v>
       </c>
-      <c r="E6" t="s" s="99">
+      <c r="E6" t="s" s="95">
         <v>74</v>
       </c>
-      <c r="F6" t="s" s="96">
+      <c r="F6" t="s" s="92">
         <v>94</v>
       </c>
     </row>
@@ -4167,19 +4150,19 @@
       <c r="A7" t="s" s="39">
         <v>101</v>
       </c>
-      <c r="B7" t="s" s="100">
+      <c r="B7" t="s" s="96">
         <v>39</v>
       </c>
       <c r="C7" t="s" s="39">
         <v>50</v>
       </c>
-      <c r="D7" t="s" s="94">
+      <c r="D7" t="s" s="90">
         <v>57</v>
       </c>
-      <c r="E7" t="s" s="99">
+      <c r="E7" t="s" s="95">
         <v>75</v>
       </c>
-      <c r="F7" t="s" s="96">
+      <c r="F7" t="s" s="92">
         <v>94</v>
       </c>
     </row>
@@ -4187,19 +4170,19 @@
       <c r="A8" t="s" s="39">
         <v>102</v>
       </c>
-      <c r="B8" t="s" s="101">
+      <c r="B8" t="s" s="97">
         <v>40</v>
       </c>
       <c r="C8" t="s" s="39">
         <v>50</v>
       </c>
-      <c r="D8" t="s" s="94">
+      <c r="D8" t="s" s="90">
         <v>57</v>
       </c>
-      <c r="E8" t="s" s="99">
+      <c r="E8" t="s" s="95">
         <v>76</v>
       </c>
-      <c r="F8" t="s" s="96">
+      <c r="F8" t="s" s="92">
         <v>94</v>
       </c>
     </row>
@@ -4207,39 +4190,39 @@
       <c r="A9" t="s" s="39">
         <v>103</v>
       </c>
-      <c r="B9" t="s" s="101">
+      <c r="B9" t="s" s="97">
         <v>41</v>
       </c>
       <c r="C9" t="s" s="39">
         <v>50</v>
       </c>
-      <c r="D9" t="s" s="94">
+      <c r="D9" t="s" s="90">
         <v>57</v>
       </c>
-      <c r="E9" t="s" s="99">
+      <c r="E9" t="s" s="95">
         <v>78</v>
       </c>
-      <c r="F9" t="s" s="96">
+      <c r="F9" t="s" s="92">
         <v>94</v>
       </c>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" t="s" s="97">
+      <c r="A10" t="s" s="93">
         <v>104</v>
       </c>
-      <c r="B10" t="s" s="98">
+      <c r="B10" t="s" s="94">
         <v>38</v>
       </c>
       <c r="C10" t="s" s="39">
         <v>49</v>
       </c>
-      <c r="D10" t="s" s="94">
+      <c r="D10" t="s" s="90">
         <v>57</v>
       </c>
-      <c r="E10" t="s" s="99">
+      <c r="E10" t="s" s="95">
         <v>74</v>
       </c>
-      <c r="F10" t="s" s="96">
+      <c r="F10" t="s" s="92">
         <v>94</v>
       </c>
     </row>
@@ -4247,19 +4230,19 @@
       <c r="A11" t="s" s="39">
         <v>105</v>
       </c>
-      <c r="B11" t="s" s="100">
+      <c r="B11" t="s" s="96">
         <v>39</v>
       </c>
       <c r="C11" t="s" s="39">
         <v>49</v>
       </c>
-      <c r="D11" t="s" s="94">
+      <c r="D11" t="s" s="90">
         <v>57</v>
       </c>
-      <c r="E11" t="s" s="99">
+      <c r="E11" t="s" s="95">
         <v>75</v>
       </c>
-      <c r="F11" t="s" s="96">
+      <c r="F11" t="s" s="92">
         <v>94</v>
       </c>
     </row>
@@ -4267,19 +4250,19 @@
       <c r="A12" t="s" s="39">
         <v>106</v>
       </c>
-      <c r="B12" t="s" s="101">
+      <c r="B12" t="s" s="97">
         <v>40</v>
       </c>
       <c r="C12" t="s" s="39">
         <v>49</v>
       </c>
-      <c r="D12" t="s" s="94">
+      <c r="D12" t="s" s="90">
         <v>57</v>
       </c>
-      <c r="E12" t="s" s="99">
+      <c r="E12" t="s" s="95">
         <v>76</v>
       </c>
-      <c r="F12" t="s" s="96">
+      <c r="F12" t="s" s="92">
         <v>94</v>
       </c>
     </row>
@@ -4287,19 +4270,19 @@
       <c r="A13" t="s" s="39">
         <v>107</v>
       </c>
-      <c r="B13" t="s" s="101">
+      <c r="B13" t="s" s="97">
         <v>41</v>
       </c>
       <c r="C13" t="s" s="39">
         <v>49</v>
       </c>
-      <c r="D13" t="s" s="94">
+      <c r="D13" t="s" s="90">
         <v>57</v>
       </c>
-      <c r="E13" t="s" s="99">
+      <c r="E13" t="s" s="95">
         <v>78</v>
       </c>
-      <c r="F13" t="s" s="96">
+      <c r="F13" t="s" s="92">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Combined ToF shutters created
</commit_message>
<xml_diff>
--- a/data/photonic_simul_data.xlsx
+++ b/data/photonic_simul_data.xlsx
@@ -11,13 +11,14 @@
     <sheet name="Lens" sheetId="4" r:id="rId7"/>
     <sheet name="Sensor" sheetId="5" r:id="rId8"/>
     <sheet name="Op" sheetId="6" r:id="rId9"/>
-    <sheet name="Config" sheetId="7" r:id="rId10"/>
+    <sheet name="WP" sheetId="7" r:id="rId10"/>
+    <sheet name="Config" sheetId="8" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -343,25 +344,25 @@
     <t>BurstTime_s</t>
   </si>
   <si>
-    <t>light_rise_sec</t>
-  </si>
-  <si>
-    <t>light_fall_sec</t>
-  </si>
-  <si>
-    <t>light_width_sec</t>
-  </si>
-  <si>
-    <t>shutter_rise_sec</t>
-  </si>
-  <si>
-    <t>shutter_fall_sec</t>
-  </si>
-  <si>
-    <t>shutter_width_sec</t>
-  </si>
-  <si>
-    <t>shutter_delay_sec</t>
+    <t>light_rise_nsec</t>
+  </si>
+  <si>
+    <t>light_fall_nsec</t>
+  </si>
+  <si>
+    <t>light_width_nsec</t>
+  </si>
+  <si>
+    <t>shutter_rise_nsec</t>
+  </si>
+  <si>
+    <t>shutter_fall_nsec</t>
+  </si>
+  <si>
+    <t>shutter_width_nsec</t>
+  </si>
+  <si>
+    <t>shutter_delay_nsec</t>
   </si>
   <si>
     <t>CW_30fps</t>
@@ -374,6 +375,21 @@
   </si>
   <si>
     <t>fake_tof</t>
+  </si>
+  <si>
+    <t>WP</t>
+  </si>
+  <si>
+    <t>ToF Working Point Table</t>
+  </si>
+  <si>
+    <t>SH1</t>
+  </si>
+  <si>
+    <t>SH2</t>
+  </si>
+  <si>
+    <t>SH3</t>
   </si>
   <si>
     <t>Configurations Table</t>
@@ -1079,7 +1095,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="98">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1336,6 +1352,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="61" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -2668,7 +2687,7 @@
     </row>
     <row r="21">
       <c r="B21" t="s" s="3">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2679,6 +2698,22 @@
         <v>5</v>
       </c>
       <c r="D22" t="s" s="5">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="B23" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24">
+      <c r="B24" s="4"/>
+      <c r="C24" t="s" s="4">
+        <v>5</v>
+      </c>
+      <c r="D24" t="s" s="5">
         <v>16</v>
       </c>
     </row>
@@ -2700,7 +2735,8 @@
     <hyperlink ref="D16" location="'Lens'!R1C1" tooltip="" display="Lens"/>
     <hyperlink ref="D18" location="'Sensor'!R1C1" tooltip="" display="Sensor"/>
     <hyperlink ref="D20" location="'Op'!R1C1" tooltip="" display="Op"/>
-    <hyperlink ref="D22" location="'Config'!R1C1" tooltip="" display="Config"/>
+    <hyperlink ref="D22" location="'WP'!R1C1" tooltip="" display="WP"/>
+    <hyperlink ref="D24" location="'Config'!R1C1" tooltip="" display="Config"/>
   </hyperlinks>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -3894,25 +3930,25 @@
         <v>0.00333333333333333</v>
       </c>
       <c r="F5" s="83">
-        <v>3e-09</v>
+        <v>3</v>
       </c>
       <c r="G5" s="83">
-        <v>5e-09</v>
+        <v>3</v>
       </c>
       <c r="H5" s="84">
-        <v>1e-08</v>
+        <v>10</v>
       </c>
       <c r="I5" s="83">
-        <v>1e-09</v>
+        <v>1</v>
       </c>
       <c r="J5" s="83">
-        <v>1e-09</v>
+        <v>1</v>
       </c>
       <c r="K5" s="84">
-        <v>1e-08</v>
+        <v>8</v>
       </c>
       <c r="L5" s="85">
-        <v>3e-09</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
@@ -4026,19 +4062,159 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
+  <dimension ref="A1:E11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col min="1" max="5" width="16.3516" style="86" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="86" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25.65" customHeight="1">
+      <c r="A1" t="s" s="63">
+        <v>96</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="30"/>
+    </row>
+    <row r="2" ht="20.45" customHeight="1">
+      <c r="A2" t="s" s="31">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s" s="32">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s" s="32">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s" s="32">
+        <v>53</v>
+      </c>
+      <c r="E2" t="s" s="33">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" ht="20.45" customHeight="1">
+      <c r="A3" t="s" s="34">
+        <v>97</v>
+      </c>
+      <c r="B3" s="35">
+        <v>2</v>
+      </c>
+      <c r="C3" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="D3" s="70">
+        <v>0.005</v>
+      </c>
+      <c r="E3" s="71">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" ht="20.2" customHeight="1">
+      <c r="A4" t="s" s="39">
+        <v>98</v>
+      </c>
+      <c r="B4" s="40">
+        <v>2.4</v>
+      </c>
+      <c r="C4" s="41">
+        <v>0.9</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
+    </row>
+    <row r="5" ht="20.2" customHeight="1">
+      <c r="A5" t="s" s="39">
+        <v>99</v>
+      </c>
+      <c r="B5" s="40">
+        <v>1.4</v>
+      </c>
+      <c r="C5" s="41">
+        <v>0.9</v>
+      </c>
+      <c r="D5" s="42"/>
+      <c r="E5" s="45">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" ht="20.2" customHeight="1">
+      <c r="A6" s="65"/>
+      <c r="B6" s="66"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43"/>
+    </row>
+    <row r="7" ht="20.2" customHeight="1">
+      <c r="A7" s="65"/>
+      <c r="B7" s="66"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43"/>
+    </row>
+    <row r="8" ht="20.2" customHeight="1">
+      <c r="A8" s="65"/>
+      <c r="B8" s="66"/>
+      <c r="C8" s="42"/>
+      <c r="D8" s="42"/>
+      <c r="E8" s="43"/>
+    </row>
+    <row r="9" ht="20.2" customHeight="1">
+      <c r="A9" s="65"/>
+      <c r="B9" s="66"/>
+      <c r="C9" s="42"/>
+      <c r="D9" s="42"/>
+      <c r="E9" s="43"/>
+    </row>
+    <row r="10" ht="20.2" customHeight="1">
+      <c r="A10" s="65"/>
+      <c r="B10" s="66"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42"/>
+      <c r="E10" s="43"/>
+    </row>
+    <row r="11" ht="20.2" customHeight="1">
+      <c r="A11" s="67"/>
+      <c r="B11" s="68"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="54"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:E1"/>
+  </mergeCells>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
+  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <headerFooter>
+    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="86" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="86" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="87" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="87" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" t="s" s="63">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -4068,221 +4244,221 @@
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>96</v>
-      </c>
-      <c r="B3" t="s" s="87">
+        <v>101</v>
+      </c>
+      <c r="B3" t="s" s="88">
         <v>29</v>
       </c>
-      <c r="C3" t="s" s="88">
+      <c r="C3" t="s" s="89">
         <v>46</v>
       </c>
       <c r="D3" t="s" s="75">
         <v>55</v>
       </c>
-      <c r="E3" t="s" s="88">
+      <c r="E3" t="s" s="89">
         <v>71</v>
       </c>
-      <c r="F3" t="s" s="89">
+      <c r="F3" t="s" s="90">
         <v>91</v>
       </c>
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="39">
-        <v>97</v>
-      </c>
-      <c r="B4" t="s" s="90">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s" s="91">
         <v>30</v>
       </c>
-      <c r="C4" t="s" s="91">
-        <v>98</v>
+      <c r="C4" t="s" s="92">
+        <v>103</v>
       </c>
       <c r="D4" t="s" s="81">
         <v>56</v>
       </c>
-      <c r="E4" t="s" s="91">
+      <c r="E4" t="s" s="92">
         <v>73</v>
       </c>
-      <c r="F4" t="s" s="92">
+      <c r="F4" t="s" s="93">
         <v>92</v>
       </c>
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="39">
-        <v>99</v>
-      </c>
-      <c r="B5" t="s" s="90">
+        <v>104</v>
+      </c>
+      <c r="B5" t="s" s="91">
         <v>29</v>
       </c>
-      <c r="C5" t="s" s="91">
+      <c r="C5" t="s" s="92">
         <v>48</v>
       </c>
       <c r="D5" t="s" s="81">
         <v>55</v>
       </c>
-      <c r="E5" t="s" s="91">
+      <c r="E5" t="s" s="92">
         <v>71</v>
       </c>
-      <c r="F5" t="s" s="92">
+      <c r="F5" t="s" s="93">
         <v>93</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="93">
-        <v>100</v>
-      </c>
-      <c r="B6" t="s" s="94">
+      <c r="A6" t="s" s="94">
+        <v>105</v>
+      </c>
+      <c r="B6" t="s" s="95">
         <v>38</v>
       </c>
       <c r="C6" t="s" s="39">
         <v>50</v>
       </c>
-      <c r="D6" t="s" s="90">
+      <c r="D6" t="s" s="91">
         <v>57</v>
       </c>
-      <c r="E6" t="s" s="95">
+      <c r="E6" t="s" s="96">
         <v>74</v>
       </c>
-      <c r="F6" t="s" s="92">
+      <c r="F6" t="s" s="93">
         <v>94</v>
       </c>
     </row>
     <row r="7" ht="20.2" customHeight="1">
       <c r="A7" t="s" s="39">
-        <v>101</v>
-      </c>
-      <c r="B7" t="s" s="96">
+        <v>106</v>
+      </c>
+      <c r="B7" t="s" s="97">
         <v>39</v>
       </c>
       <c r="C7" t="s" s="39">
         <v>50</v>
       </c>
-      <c r="D7" t="s" s="90">
+      <c r="D7" t="s" s="91">
         <v>57</v>
       </c>
-      <c r="E7" t="s" s="95">
+      <c r="E7" t="s" s="96">
         <v>75</v>
       </c>
-      <c r="F7" t="s" s="92">
+      <c r="F7" t="s" s="93">
         <v>94</v>
       </c>
     </row>
     <row r="8" ht="20.2" customHeight="1">
       <c r="A8" t="s" s="39">
-        <v>102</v>
-      </c>
-      <c r="B8" t="s" s="97">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s" s="98">
         <v>40</v>
       </c>
       <c r="C8" t="s" s="39">
         <v>50</v>
       </c>
-      <c r="D8" t="s" s="90">
+      <c r="D8" t="s" s="91">
         <v>57</v>
       </c>
-      <c r="E8" t="s" s="95">
+      <c r="E8" t="s" s="96">
         <v>76</v>
       </c>
-      <c r="F8" t="s" s="92">
+      <c r="F8" t="s" s="93">
         <v>94</v>
       </c>
     </row>
     <row r="9" ht="20.2" customHeight="1">
       <c r="A9" t="s" s="39">
-        <v>103</v>
-      </c>
-      <c r="B9" t="s" s="97">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s" s="98">
         <v>41</v>
       </c>
       <c r="C9" t="s" s="39">
         <v>50</v>
       </c>
-      <c r="D9" t="s" s="90">
+      <c r="D9" t="s" s="91">
         <v>57</v>
       </c>
-      <c r="E9" t="s" s="95">
+      <c r="E9" t="s" s="96">
         <v>78</v>
       </c>
-      <c r="F9" t="s" s="92">
+      <c r="F9" t="s" s="93">
         <v>94</v>
       </c>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" t="s" s="93">
-        <v>104</v>
-      </c>
-      <c r="B10" t="s" s="94">
+      <c r="A10" t="s" s="94">
+        <v>109</v>
+      </c>
+      <c r="B10" t="s" s="95">
         <v>38</v>
       </c>
       <c r="C10" t="s" s="39">
         <v>49</v>
       </c>
-      <c r="D10" t="s" s="90">
+      <c r="D10" t="s" s="91">
         <v>57</v>
       </c>
-      <c r="E10" t="s" s="95">
+      <c r="E10" t="s" s="96">
         <v>74</v>
       </c>
-      <c r="F10" t="s" s="92">
+      <c r="F10" t="s" s="93">
         <v>94</v>
       </c>
     </row>
     <row r="11" ht="20.2" customHeight="1">
       <c r="A11" t="s" s="39">
-        <v>105</v>
-      </c>
-      <c r="B11" t="s" s="96">
+        <v>110</v>
+      </c>
+      <c r="B11" t="s" s="97">
         <v>39</v>
       </c>
       <c r="C11" t="s" s="39">
         <v>49</v>
       </c>
-      <c r="D11" t="s" s="90">
+      <c r="D11" t="s" s="91">
         <v>57</v>
       </c>
-      <c r="E11" t="s" s="95">
+      <c r="E11" t="s" s="96">
         <v>75</v>
       </c>
-      <c r="F11" t="s" s="92">
+      <c r="F11" t="s" s="93">
         <v>94</v>
       </c>
     </row>
     <row r="12" ht="20.2" customHeight="1">
       <c r="A12" t="s" s="39">
-        <v>106</v>
-      </c>
-      <c r="B12" t="s" s="97">
+        <v>111</v>
+      </c>
+      <c r="B12" t="s" s="98">
         <v>40</v>
       </c>
       <c r="C12" t="s" s="39">
         <v>49</v>
       </c>
-      <c r="D12" t="s" s="90">
+      <c r="D12" t="s" s="91">
         <v>57</v>
       </c>
-      <c r="E12" t="s" s="95">
+      <c r="E12" t="s" s="96">
         <v>76</v>
       </c>
-      <c r="F12" t="s" s="92">
+      <c r="F12" t="s" s="93">
         <v>94</v>
       </c>
     </row>
     <row r="13" ht="20.2" customHeight="1">
       <c r="A13" t="s" s="39">
-        <v>107</v>
-      </c>
-      <c r="B13" t="s" s="97">
+        <v>112</v>
+      </c>
+      <c r="B13" t="s" s="98">
         <v>41</v>
       </c>
       <c r="C13" t="s" s="39">
         <v>49</v>
       </c>
-      <c r="D13" t="s" s="90">
+      <c r="D13" t="s" s="91">
         <v>57</v>
       </c>
-      <c r="E13" t="s" s="95">
+      <c r="E13" t="s" s="96">
         <v>78</v>
       </c>
-      <c r="F13" t="s" s="92">
+      <c r="F13" t="s" s="93">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add ToF depth error simulation by Monte Carlo
</commit_message>
<xml_diff>
--- a/data/photonic_simul_data.xlsx
+++ b/data/photonic_simul_data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -399,9 +399,6 @@
   </si>
   <si>
     <t>Cfg2</t>
-  </si>
-  <si>
-    <t>Room_4</t>
   </si>
   <si>
     <t>Cfg3</t>
@@ -2823,7 +2820,7 @@
         <v>60</v>
       </c>
       <c r="F3" s="36">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="G3" s="36">
         <v>1</v>
@@ -3507,7 +3504,7 @@
         <v>71</v>
       </c>
       <c r="B3" s="74">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C3" s="36">
         <v>850</v>
@@ -3920,7 +3917,7 @@
         <v>30</v>
       </c>
       <c r="C5" s="41">
-        <v>1000</v>
+        <v>20000</v>
       </c>
       <c r="D5" s="41">
         <v>0.0036</v>
@@ -4270,7 +4267,7 @@
         <v>30</v>
       </c>
       <c r="C4" t="s" s="92">
-        <v>103</v>
+        <v>48</v>
       </c>
       <c r="D4" t="s" s="81">
         <v>56</v>
@@ -4284,16 +4281,16 @@
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="39">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s" s="91">
         <v>29</v>
       </c>
       <c r="C5" t="s" s="92">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="D5" t="s" s="81">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s" s="92">
         <v>71</v>
@@ -4304,7 +4301,7 @@
     </row>
     <row r="6" ht="20.2" customHeight="1">
       <c r="A6" t="s" s="94">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s" s="95">
         <v>38</v>
@@ -4324,7 +4321,7 @@
     </row>
     <row r="7" ht="20.2" customHeight="1">
       <c r="A7" t="s" s="39">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s" s="97">
         <v>39</v>
@@ -4344,7 +4341,7 @@
     </row>
     <row r="8" ht="20.2" customHeight="1">
       <c r="A8" t="s" s="39">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s" s="98">
         <v>40</v>
@@ -4364,7 +4361,7 @@
     </row>
     <row r="9" ht="20.2" customHeight="1">
       <c r="A9" t="s" s="39">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B9" t="s" s="98">
         <v>41</v>
@@ -4384,7 +4381,7 @@
     </row>
     <row r="10" ht="20.2" customHeight="1">
       <c r="A10" t="s" s="94">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B10" t="s" s="95">
         <v>38</v>
@@ -4404,7 +4401,7 @@
     </row>
     <row r="11" ht="20.2" customHeight="1">
       <c r="A11" t="s" s="39">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B11" t="s" s="97">
         <v>39</v>
@@ -4424,7 +4421,7 @@
     </row>
     <row r="12" ht="20.2" customHeight="1">
       <c r="A12" t="s" s="39">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B12" t="s" s="98">
         <v>40</v>
@@ -4444,7 +4441,7 @@
     </row>
     <row r="13" ht="20.2" customHeight="1">
       <c r="A13" t="s" s="39">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B13" t="s" s="98">
         <v>41</v>

</xml_diff>

<commit_message>
Add power consumption and heat dissipation
</commit_message>
<xml_diff>
--- a/data/photonic_simul_data.xlsx
+++ b/data/photonic_simul_data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -203,6 +203,20 @@
     </r>
   </si>
   <si>
+    <t>SPL_UL90AT08</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>https://www.osram.com/ecat/Metal%20Can%C2%AE%20TO56%20SPL%20UL90AT08/com/en/class_pim_web_catalog_103489/global/prd_pim_device_2220021/</t>
+    </r>
+  </si>
+  <si>
     <t>MCM-124</t>
   </si>
   <si>
@@ -236,6 +250,9 @@
     <t>Road_Day_60</t>
   </si>
   <si>
+    <t>Road_day_200</t>
+  </si>
+  <si>
     <t>Road_night_200</t>
   </si>
   <si>
@@ -266,6 +283,9 @@
     <t>fake_tof_lens</t>
   </si>
   <si>
+    <t>Lidar_lens</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sensor Table </t>
   </si>
   <si>
@@ -305,6 +325,9 @@
     <t>CDS</t>
   </si>
   <si>
+    <t>Power_nJ_pix</t>
+  </si>
+  <si>
     <t>Sensor1_850</t>
   </si>
   <si>
@@ -329,9 +352,15 @@
     <t>ToF_1550</t>
   </si>
   <si>
+    <t>Lidar_PIN_detector</t>
+  </si>
+  <si>
     <t>Operational Modes Table</t>
   </si>
   <si>
+    <t>image_mode</t>
+  </si>
+  <si>
     <t>frame_rate</t>
   </si>
   <si>
@@ -344,6 +373,12 @@
     <t>BurstTime_s</t>
   </si>
   <si>
+    <t>integTime_s</t>
+  </si>
+  <si>
+    <t>N_subframes</t>
+  </si>
+  <si>
     <t>light_rise_nsec</t>
   </si>
   <si>
@@ -368,21 +403,33 @@
     <t>CW_30fps</t>
   </si>
   <si>
+    <t>Camera</t>
+  </si>
+  <si>
     <t>CW_60fps</t>
   </si>
   <si>
-    <t>pls_30_1000</t>
+    <t>pls_30_20000</t>
   </si>
   <si>
     <t>fake_tof</t>
   </si>
   <si>
+    <t>Lidar2_60fps</t>
+  </si>
+  <si>
+    <t>Lidar_2_ax</t>
+  </si>
+  <si>
     <t>WP</t>
   </si>
   <si>
     <t>ToF Working Point Table</t>
   </si>
   <si>
+    <t>N.instances</t>
+  </si>
+  <si>
     <t>SH1</t>
   </si>
   <si>
@@ -402,6 +449,9 @@
   </si>
   <si>
     <t>Cfg3</t>
+  </si>
+  <si>
+    <t>Lidar_2_axes</t>
   </si>
   <si>
     <t>fake_tof_night_850</t>
@@ -539,7 +589,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="45">
     <border>
       <left/>
       <right/>
@@ -1028,6 +1078,51 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="18"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="8"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top style="thin">
+        <color indexed="18"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="16"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color indexed="16"/>
       </left>
       <right style="thin">
@@ -1092,7 +1187,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1204,9 +1299,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1321,6 +1413,9 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1342,6 +1437,15 @@
     <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="61" fontId="0" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="61" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1351,9 +1455,21 @@
     <xf numFmtId="61" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="17" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1375,19 +1491,22 @@
     <xf numFmtId="49" fontId="7" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="6" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="43" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="44" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2684,7 +2803,7 @@
     </row>
     <row r="21">
       <c r="B21" t="s" s="3">
-        <v>95</v>
+        <v>107</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2695,7 +2814,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s" s="5">
-        <v>95</v>
+        <v>107</v>
       </c>
     </row>
     <row r="23">
@@ -2745,7 +2864,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -2823,305 +2942,342 @@
         <v>40</v>
       </c>
       <c r="G3" s="36">
+        <v>2</v>
+      </c>
+      <c r="H3" s="36">
+        <v>4</v>
+      </c>
+      <c r="I3" s="36">
+        <v>8</v>
+      </c>
+      <c r="J3" s="37"/>
+    </row>
+    <row r="4" ht="20.2" customHeight="1">
+      <c r="A4" t="s" s="38">
+        <v>30</v>
+      </c>
+      <c r="B4" s="39">
+        <v>10</v>
+      </c>
+      <c r="C4" s="40">
+        <v>940</v>
+      </c>
+      <c r="D4" s="40">
+        <v>0.95</v>
+      </c>
+      <c r="E4" s="40">
+        <v>60</v>
+      </c>
+      <c r="F4" s="40">
+        <v>60</v>
+      </c>
+      <c r="G4" s="40">
         <v>1</v>
       </c>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="38"/>
-    </row>
-    <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="39">
-        <v>30</v>
-      </c>
-      <c r="B4" s="40">
-        <v>10</v>
-      </c>
-      <c r="C4" s="41">
-        <v>940</v>
-      </c>
-      <c r="D4" s="41">
+      <c r="H4" s="41"/>
+      <c r="I4" s="41"/>
+      <c r="J4" s="42"/>
+    </row>
+    <row r="5" ht="20.2" customHeight="1">
+      <c r="A5" t="s" s="38">
+        <v>31</v>
+      </c>
+      <c r="B5" s="39">
+        <v>2.1</v>
+      </c>
+      <c r="C5" s="40">
+        <v>1550</v>
+      </c>
+      <c r="D5" s="40">
         <v>0.95</v>
       </c>
-      <c r="E4" s="41">
-        <v>60</v>
-      </c>
-      <c r="F4" s="41">
-        <v>60</v>
-      </c>
-      <c r="G4" s="41">
+      <c r="E5" s="40">
+        <v>40</v>
+      </c>
+      <c r="F5" s="40">
+        <v>20</v>
+      </c>
+      <c r="G5" s="40">
+        <v>4</v>
+      </c>
+      <c r="H5" s="40">
+        <v>1.9</v>
+      </c>
+      <c r="I5" s="40">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s" s="43">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" ht="20.2" customHeight="1">
+      <c r="A6" t="s" s="38">
+        <v>33</v>
+      </c>
+      <c r="B6" s="39">
+        <v>20</v>
+      </c>
+      <c r="C6" s="40">
+        <v>1550</v>
+      </c>
+      <c r="D6" s="40">
+        <v>0.95</v>
+      </c>
+      <c r="E6" s="40">
+        <v>40</v>
+      </c>
+      <c r="F6" s="40">
+        <v>20</v>
+      </c>
+      <c r="G6" s="40">
         <v>1</v>
       </c>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="43"/>
-    </row>
-    <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="39">
-        <v>31</v>
-      </c>
-      <c r="B5" s="40">
-        <v>2.1</v>
-      </c>
-      <c r="C5" s="41">
-        <v>1550</v>
-      </c>
-      <c r="D5" s="41">
-        <v>0.95</v>
-      </c>
-      <c r="E5" s="41">
-        <v>40</v>
-      </c>
-      <c r="F5" s="41">
-        <v>20</v>
-      </c>
-      <c r="G5" s="41">
-        <v>4</v>
-      </c>
-      <c r="H5" s="41">
-        <v>1.9</v>
-      </c>
-      <c r="I5" s="41">
-        <v>6</v>
-      </c>
-      <c r="J5" t="s" s="44">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="39">
-        <v>33</v>
-      </c>
-      <c r="B6" s="40">
-        <v>20</v>
-      </c>
-      <c r="C6" s="41">
-        <v>1550</v>
-      </c>
-      <c r="D6" s="41">
-        <v>0.95</v>
-      </c>
-      <c r="E6" s="41">
-        <v>40</v>
-      </c>
-      <c r="F6" s="41">
-        <v>20</v>
-      </c>
-      <c r="G6" s="41">
-        <v>1</v>
-      </c>
-      <c r="H6" s="41">
+      <c r="H6" s="40">
         <v>10.7</v>
       </c>
-      <c r="I6" s="41">
+      <c r="I6" s="40">
         <f>B6/2.2</f>
         <v>9.09090909090909</v>
       </c>
-      <c r="J6" t="s" s="44">
+      <c r="J6" t="s" s="43">
         <v>34</v>
       </c>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" t="s" s="39">
+      <c r="A7" t="s" s="38">
         <v>35</v>
       </c>
-      <c r="B7" s="40">
+      <c r="B7" s="39">
         <v>4</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="40">
         <v>940</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D7" s="40">
         <v>0.95</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="40">
         <v>40</v>
       </c>
-      <c r="F7" s="45">
+      <c r="F7" s="44">
         <v>20</v>
       </c>
-      <c r="G7" s="46">
+      <c r="G7" s="45">
         <v>1</v>
       </c>
-      <c r="H7" s="41">
+      <c r="H7" s="40">
         <v>2</v>
       </c>
-      <c r="I7" s="41">
+      <c r="I7" s="40">
         <v>6</v>
       </c>
-      <c r="J7" t="s" s="44">
+      <c r="J7" t="s" s="43">
         <v>36</v>
       </c>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" t="s" s="39">
+      <c r="A8" t="s" s="38">
         <v>37</v>
       </c>
-      <c r="B8" s="40">
+      <c r="B8" s="39">
+        <v>125</v>
+      </c>
+      <c r="C8" s="40">
+        <v>905</v>
+      </c>
+      <c r="D8" s="40">
+        <v>0.95</v>
+      </c>
+      <c r="E8" s="40">
+        <v>0.1</v>
+      </c>
+      <c r="F8" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="G8" s="45">
+        <v>1</v>
+      </c>
+      <c r="H8" s="40">
+        <v>11</v>
+      </c>
+      <c r="I8" s="40">
+        <v>38</v>
+      </c>
+      <c r="J8" t="s" s="43">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" ht="20.2" customHeight="1">
+      <c r="A9" t="s" s="38">
+        <v>39</v>
+      </c>
+      <c r="B9" s="39">
         <v>28</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C9" s="46">
         <v>1375</v>
       </c>
-      <c r="D8" s="41">
+      <c r="D9" s="40">
         <v>0.95</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E9" s="40">
         <v>40</v>
       </c>
-      <c r="F8" s="41">
+      <c r="F9" s="40">
         <v>20</v>
       </c>
-      <c r="G8" s="41">
+      <c r="G9" s="40">
         <v>1</v>
       </c>
-      <c r="H8" s="41">
+      <c r="H9" s="40">
         <v>11.5</v>
       </c>
-      <c r="I8" s="41">
+      <c r="I9" s="40">
         <v>12.5</v>
       </c>
-      <c r="J8" t="s" s="44">
+      <c r="J9" t="s" s="43">
         <v>34</v>
       </c>
     </row>
-    <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" t="s" s="39">
-        <v>38</v>
-      </c>
-      <c r="B9" s="40">
+    <row r="10" ht="20.2" customHeight="1">
+      <c r="A10" t="s" s="38">
+        <v>40</v>
+      </c>
+      <c r="B10" s="39">
         <f>50*0.5</f>
         <v>25</v>
       </c>
-      <c r="C9" s="36">
+      <c r="C10" s="36">
         <v>850</v>
       </c>
-      <c r="D9" s="41">
+      <c r="D10" s="40">
         <v>0.95</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E10" s="40">
         <v>70</v>
       </c>
-      <c r="F9" s="41">
+      <c r="F10" s="40">
         <v>60</v>
       </c>
-      <c r="G9" s="41">
+      <c r="G10" s="40">
         <v>2</v>
       </c>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="43"/>
-    </row>
-    <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" t="s" s="48">
-        <v>39</v>
-      </c>
-      <c r="B10" s="40">
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="42"/>
+    </row>
+    <row r="11" ht="20.2" customHeight="1">
+      <c r="A11" t="s" s="47">
+        <v>41</v>
+      </c>
+      <c r="B11" s="39">
         <f>50*0.38</f>
         <v>19</v>
       </c>
-      <c r="C10" s="41">
+      <c r="C11" s="40">
         <v>940</v>
       </c>
-      <c r="D10" s="41">
+      <c r="D11" s="40">
         <v>0.95</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E11" s="40">
         <v>70</v>
       </c>
-      <c r="F10" s="41">
+      <c r="F11" s="40">
         <v>60</v>
       </c>
-      <c r="G10" s="41">
+      <c r="G11" s="40">
         <v>2</v>
       </c>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="43"/>
-    </row>
-    <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" t="s" s="49">
-        <v>40</v>
-      </c>
-      <c r="B11" s="40">
+      <c r="H11" s="41"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="42"/>
+    </row>
+    <row r="12" ht="20.2" customHeight="1">
+      <c r="A12" t="s" s="48">
+        <v>42</v>
+      </c>
+      <c r="B12" s="39">
         <f>50*0.22</f>
         <v>11</v>
       </c>
-      <c r="C11" s="41">
+      <c r="C12" s="40">
         <v>1375</v>
       </c>
-      <c r="D11" s="41">
+      <c r="D12" s="40">
         <v>0.95</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E12" s="40">
         <v>70</v>
       </c>
-      <c r="F11" s="41">
+      <c r="F12" s="40">
         <v>60</v>
       </c>
-      <c r="G11" s="41">
+      <c r="G12" s="40">
         <v>2</v>
       </c>
-      <c r="H11" s="42"/>
-      <c r="I11" s="42"/>
-      <c r="J11" s="43"/>
-    </row>
-    <row r="12" ht="20.2" customHeight="1">
-      <c r="A12" t="s" s="50">
-        <v>41</v>
-      </c>
-      <c r="B12" s="51">
-        <f>50*0.19+C14</f>
+      <c r="H12" s="41"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="42"/>
+    </row>
+    <row r="13" ht="20.2" customHeight="1">
+      <c r="A13" t="s" s="49">
+        <v>43</v>
+      </c>
+      <c r="B13" s="50">
+        <f>50*0.19+C15</f>
         <v>9.5</v>
       </c>
-      <c r="C12" s="41">
+      <c r="C13" s="40">
         <v>1550</v>
       </c>
-      <c r="D12" s="52">
+      <c r="D13" s="51">
         <v>0.95</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E13" s="51">
         <v>70</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F13" s="51">
         <v>60</v>
       </c>
-      <c r="G12" s="52">
+      <c r="G13" s="51">
         <v>2</v>
       </c>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="54"/>
-    </row>
-    <row r="13" ht="14.7" customHeight="1">
-      <c r="A13" s="55"/>
-      <c r="B13" s="56"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="56"/>
-      <c r="E13" s="56"/>
-      <c r="F13" s="56"/>
-      <c r="G13" s="56"/>
-      <c r="H13" s="56"/>
-      <c r="I13" s="56"/>
-      <c r="J13" s="58"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
     </row>
     <row r="14" ht="14.7" customHeight="1">
-      <c r="A14" s="59"/>
-      <c r="B14" s="60"/>
-      <c r="C14" s="60"/>
-      <c r="D14" s="60"/>
-      <c r="E14" s="60"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="60"/>
-      <c r="H14" s="60"/>
-      <c r="I14" s="60"/>
-      <c r="J14" s="61"/>
+      <c r="A14" s="54"/>
+      <c r="B14" s="55"/>
+      <c r="C14" s="56"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="55"/>
+      <c r="J14" s="57"/>
+    </row>
+    <row r="15" ht="14.7" customHeight="1">
+      <c r="A15" s="58"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="59"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="60"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="J5" r:id="rId1" location="" tooltip="" display="https://www.thorlabs.com/drawings/471c86010a0aa6dc-F53DE964-0AE3-E9AF-406B86F1AA7C426E/L1550G1-SpecSheet.pdf"/>
     <hyperlink ref="J6" r:id="rId2" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
     <hyperlink ref="J7" r:id="rId3" location="" tooltip="" display="https://www.ii-vi.com/wp-content/uploads/2019/07/940nm-Multi-Mode-High-Power-VCSEL-Array-web-2-1.pdf"/>
-    <hyperlink ref="J8" r:id="rId4" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
+    <hyperlink ref="J8" r:id="rId4" location="" tooltip="" display="https://www.osram.com/ecat/Metal%20Can%C2%AE%20TO56%20SPL%20UL90AT08/com/en/class_pim_web_catalog_103489/global/prd_pim_device_2220021/"/>
+    <hyperlink ref="J9" r:id="rId5" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -3136,19 +3292,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="62" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="62" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="61" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="61" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="63">
-        <v>42</v>
+      <c r="A1" t="s" s="62">
+        <v>44</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -3160,19 +3316,19 @@
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C2" t="s" s="32">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s" s="32">
-        <v>45</v>
-      </c>
-      <c r="E2" s="64"/>
+        <v>47</v>
+      </c>
+      <c r="E2" s="63"/>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B3" s="35">
         <v>3</v>
@@ -3183,95 +3339,110 @@
       <c r="D3" s="36">
         <v>1000</v>
       </c>
-      <c r="E3" s="38"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="39">
-        <v>47</v>
-      </c>
-      <c r="B4" s="40">
+      <c r="A4" t="s" s="38">
+        <v>49</v>
+      </c>
+      <c r="B4" s="39">
         <v>60</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="40">
         <v>0.5</v>
       </c>
-      <c r="D4" s="41">
+      <c r="D4" s="40">
         <v>30000</v>
       </c>
-      <c r="E4" s="43"/>
+      <c r="E4" s="42"/>
     </row>
     <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="39">
-        <v>48</v>
-      </c>
-      <c r="B5" s="40">
+      <c r="A5" t="s" s="38">
+        <v>50</v>
+      </c>
+      <c r="B5" s="39">
         <v>200</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="40">
         <v>0.5</v>
       </c>
-      <c r="D5" s="41">
+      <c r="D5" s="40">
+        <v>100000</v>
+      </c>
+      <c r="E5" s="42"/>
+    </row>
+    <row r="6" ht="20.2" customHeight="1">
+      <c r="A6" t="s" s="38">
+        <v>51</v>
+      </c>
+      <c r="B6" s="39">
+        <v>200</v>
+      </c>
+      <c r="C6" s="40">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="40">
         <v>1</v>
       </c>
-      <c r="E5" s="43"/>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="39">
-        <v>49</v>
-      </c>
-      <c r="B6" s="40">
+      <c r="E6" s="42"/>
+    </row>
+    <row r="7" ht="20.2" customHeight="1">
+      <c r="A7" t="s" s="38">
+        <v>52</v>
+      </c>
+      <c r="B7" s="39">
         <v>5</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C7" s="40">
         <v>0.5</v>
       </c>
-      <c r="D6" s="41">
+      <c r="D7" s="40">
         <v>100000</v>
       </c>
-      <c r="E6" s="43"/>
-    </row>
-    <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" t="s" s="39">
-        <v>50</v>
-      </c>
-      <c r="B7" s="40">
+      <c r="E7" s="42"/>
+    </row>
+    <row r="8" ht="20.2" customHeight="1">
+      <c r="A8" t="s" s="38">
+        <v>53</v>
+      </c>
+      <c r="B8" s="39">
         <v>5</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C8" s="40">
         <v>0.5</v>
       </c>
-      <c r="D7" s="41">
+      <c r="D8" s="40">
         <v>0.01</v>
       </c>
-      <c r="E7" s="43"/>
-    </row>
-    <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="65"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="65"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="65"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
+      <c r="A11" s="64"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="42"/>
+    </row>
+    <row r="12" ht="20.2" customHeight="1">
+      <c r="A12" s="66"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3296,13 +3467,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="69" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="69" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="68" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="68" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="63">
-        <v>51</v>
+      <c r="A1" t="s" s="62">
+        <v>54</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -3314,21 +3485,21 @@
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s" s="32">
         <v>22</v>
       </c>
       <c r="D2" t="s" s="32">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s" s="33">
-        <v>54</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B3" s="35">
         <v>2</v>
@@ -3336,82 +3507,90 @@
       <c r="C3" s="36">
         <v>0.9</v>
       </c>
-      <c r="D3" s="70">
+      <c r="D3" s="69">
         <v>0.005</v>
       </c>
-      <c r="E3" s="71">
+      <c r="E3" s="70">
         <v>50</v>
       </c>
     </row>
     <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="39">
-        <v>56</v>
-      </c>
-      <c r="B4" s="40">
+      <c r="A4" t="s" s="38">
+        <v>59</v>
+      </c>
+      <c r="B4" s="39">
         <v>2.4</v>
       </c>
-      <c r="C4" s="41">
+      <c r="C4" s="40">
         <v>0.9</v>
       </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
     </row>
     <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="39">
-        <v>57</v>
-      </c>
-      <c r="B5" s="40">
+      <c r="A5" t="s" s="38">
+        <v>60</v>
+      </c>
+      <c r="B5" s="39">
         <v>1.4</v>
       </c>
-      <c r="C5" s="41">
+      <c r="C5" s="40">
         <v>0.9</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="45">
+      <c r="D5" s="41"/>
+      <c r="E5" s="44">
         <v>50</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" s="65"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
+      <c r="A6" t="s" s="38">
+        <v>61</v>
+      </c>
+      <c r="B6" s="39">
+        <v>1</v>
+      </c>
+      <c r="C6" s="40">
+        <v>0.9</v>
+      </c>
+      <c r="D6" s="41"/>
+      <c r="E6" s="44">
+        <v>50</v>
+      </c>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="65"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="65"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="65"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="65"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3430,21 +3609,21 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="16.3516" style="72" customWidth="1"/>
-    <col min="2" max="13" width="10.125" style="72" customWidth="1"/>
-    <col min="14" max="16384" width="16.3516" style="72" customWidth="1"/>
+    <col min="1" max="1" width="16.3516" style="71" customWidth="1"/>
+    <col min="2" max="14" width="10.125" style="71" customWidth="1"/>
+    <col min="15" max="16384" width="16.3516" style="71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" s="26"/>
       <c r="B1" t="s" s="29">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="27"/>
@@ -3456,66 +3635,70 @@
       <c r="J1" s="28"/>
       <c r="K1" s="27"/>
       <c r="L1" s="27"/>
-      <c r="M1" s="73"/>
+      <c r="M1" s="27"/>
+      <c r="N1" s="72"/>
     </row>
     <row r="2" ht="26.7" customHeight="1">
       <c r="A2" t="s" s="31">
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s" s="32">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D2" t="s" s="32">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="E2" t="s" s="32">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="F2" t="s" s="32">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G2" t="s" s="32">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="H2" t="s" s="32">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="I2" t="s" s="32">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="J2" t="s" s="32">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="K2" t="s" s="32">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="L2" t="s" s="32">
-        <v>69</v>
-      </c>
-      <c r="M2" t="s" s="33">
-        <v>70</v>
+        <v>73</v>
+      </c>
+      <c r="M2" t="s" s="32">
+        <v>74</v>
+      </c>
+      <c r="N2" t="s" s="33">
+        <v>75</v>
       </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>71</v>
-      </c>
-      <c r="B3" s="74">
+        <v>76</v>
+      </c>
+      <c r="B3" s="73">
         <v>7</v>
       </c>
       <c r="C3" s="36">
         <v>850</v>
       </c>
-      <c r="D3" t="s" s="75">
-        <v>72</v>
+      <c r="D3" t="s" s="74">
+        <v>77</v>
       </c>
       <c r="E3" s="36">
         <v>10</v>
       </c>
-      <c r="F3" s="37"/>
+      <c r="F3" s="75"/>
       <c r="G3" s="36">
         <v>0.7</v>
       </c>
@@ -3531,51 +3714,57 @@
       <c r="K3" s="36">
         <v>5000</v>
       </c>
-      <c r="L3" s="37"/>
-      <c r="M3" t="b" s="71">
+      <c r="L3" s="75"/>
+      <c r="M3" t="b" s="36">
         <v>1</v>
+      </c>
+      <c r="N3" s="70">
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="76">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="B4" s="77">
         <v>3</v>
       </c>
-      <c r="C4" s="47">
+      <c r="C4" s="46">
         <v>550</v>
       </c>
       <c r="D4" t="s" s="78">
-        <v>72</v>
-      </c>
-      <c r="E4" s="47">
+        <v>77</v>
+      </c>
+      <c r="E4" s="46">
         <v>10</v>
       </c>
       <c r="F4" s="79"/>
-      <c r="G4" s="47">
+      <c r="G4" s="46">
         <v>0.7</v>
       </c>
-      <c r="H4" s="47">
+      <c r="H4" s="46">
         <v>640</v>
       </c>
-      <c r="I4" s="47">
+      <c r="I4" s="46">
         <v>480</v>
       </c>
-      <c r="J4" s="47">
+      <c r="J4" s="46">
         <v>5</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="46">
         <v>5000</v>
       </c>
       <c r="L4" s="79"/>
-      <c r="M4" t="b" s="80">
+      <c r="M4" t="b" s="46">
         <v>1</v>
+      </c>
+      <c r="N4" s="80">
+        <v>1.5</v>
       </c>
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="34">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="B5" s="35">
         <v>7.5</v>
@@ -3583,13 +3772,13 @@
       <c r="C5" s="36">
         <v>850</v>
       </c>
-      <c r="D5" t="s" s="75">
-        <v>72</v>
+      <c r="D5" t="s" s="74">
+        <v>77</v>
       </c>
       <c r="E5" s="36">
         <v>10</v>
       </c>
-      <c r="F5" s="37"/>
+      <c r="F5" s="75"/>
       <c r="G5" s="36">
         <v>1</v>
       </c>
@@ -3608,171 +3797,200 @@
       <c r="L5" s="36">
         <v>10</v>
       </c>
-      <c r="M5" t="b" s="71">
+      <c r="M5" t="b" s="36">
         <v>0</v>
       </c>
+      <c r="N5" s="70">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="39">
-        <v>75</v>
-      </c>
-      <c r="B6" s="40">
+      <c r="A6" t="s" s="38">
+        <v>80</v>
+      </c>
+      <c r="B6" s="39">
         <v>7.5</v>
       </c>
-      <c r="C6" s="41">
+      <c r="C6" s="40">
         <v>940</v>
       </c>
       <c r="D6" t="s" s="81">
-        <v>72</v>
-      </c>
-      <c r="E6" s="41">
+        <v>77</v>
+      </c>
+      <c r="E6" s="40">
         <v>10</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="41">
+      <c r="F6" s="41"/>
+      <c r="G6" s="40">
         <v>1</v>
       </c>
-      <c r="H6" s="41">
+      <c r="H6" s="40">
         <v>640</v>
       </c>
-      <c r="I6" s="45">
+      <c r="I6" s="44">
         <v>480</v>
       </c>
-      <c r="J6" s="46">
+      <c r="J6" s="45">
         <v>5</v>
       </c>
-      <c r="K6" s="41">
+      <c r="K6" s="40">
         <v>5000</v>
       </c>
-      <c r="L6" s="41">
+      <c r="L6" s="40">
         <v>10</v>
       </c>
-      <c r="M6" t="b" s="45">
+      <c r="M6" t="b" s="40">
         <v>0</v>
       </c>
+      <c r="N6" s="44">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" t="s" s="39">
-        <v>76</v>
-      </c>
-      <c r="B7" s="40">
+      <c r="A7" t="s" s="38">
+        <v>81</v>
+      </c>
+      <c r="B7" s="39">
         <v>7.5</v>
       </c>
-      <c r="C7" s="41">
+      <c r="C7" s="40">
         <v>1375</v>
       </c>
       <c r="D7" t="s" s="81">
+        <v>82</v>
+      </c>
+      <c r="E7" s="40">
+        <v>1</v>
+      </c>
+      <c r="F7" s="41"/>
+      <c r="G7" s="40">
+        <v>1</v>
+      </c>
+      <c r="H7" s="40">
+        <v>640</v>
+      </c>
+      <c r="I7" s="44">
+        <v>480</v>
+      </c>
+      <c r="J7" s="45">
+        <v>5</v>
+      </c>
+      <c r="K7" s="40">
+        <v>5000</v>
+      </c>
+      <c r="L7" s="40">
+        <v>10</v>
+      </c>
+      <c r="M7" t="b" s="40">
+        <v>0</v>
+      </c>
+      <c r="N7" s="44">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="8" ht="20.2" customHeight="1">
+      <c r="A8" t="s" s="38">
+        <v>83</v>
+      </c>
+      <c r="B8" s="39">
+        <v>7.5</v>
+      </c>
+      <c r="C8" s="40">
+        <v>1550</v>
+      </c>
+      <c r="D8" t="s" s="81">
+        <v>82</v>
+      </c>
+      <c r="E8" s="40">
+        <v>1</v>
+      </c>
+      <c r="F8" s="41"/>
+      <c r="G8" s="40">
+        <v>1</v>
+      </c>
+      <c r="H8" s="40">
+        <v>640</v>
+      </c>
+      <c r="I8" s="40">
+        <v>480</v>
+      </c>
+      <c r="J8" s="40">
+        <v>5</v>
+      </c>
+      <c r="K8" s="40">
+        <v>5000</v>
+      </c>
+      <c r="L8" s="40">
+        <v>10</v>
+      </c>
+      <c r="M8" t="b" s="40">
+        <v>0</v>
+      </c>
+      <c r="N8" s="44">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="9" ht="20.2" customHeight="1">
+      <c r="A9" t="s" s="38">
+        <v>84</v>
+      </c>
+      <c r="B9" s="39">
+        <v>20</v>
+      </c>
+      <c r="C9" s="40">
+        <v>940</v>
+      </c>
+      <c r="D9" t="s" s="81">
         <v>77</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E9" s="40">
+        <v>30</v>
+      </c>
+      <c r="F9" s="41"/>
+      <c r="G9" s="40">
         <v>1</v>
       </c>
-      <c r="F7" s="42"/>
-      <c r="G7" s="41">
-        <v>1</v>
-      </c>
-      <c r="H7" s="41">
-        <v>640</v>
-      </c>
-      <c r="I7" s="45">
-        <v>480</v>
-      </c>
-      <c r="J7" s="46">
-        <v>5</v>
-      </c>
-      <c r="K7" s="41">
-        <v>5000</v>
-      </c>
-      <c r="L7" s="41">
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="44">
         <v>10</v>
       </c>
-      <c r="M7" t="b" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" t="s" s="39">
-        <v>78</v>
-      </c>
-      <c r="B8" s="40">
-        <v>7.5</v>
-      </c>
-      <c r="C8" s="41">
-        <v>1550</v>
-      </c>
-      <c r="D8" t="s" s="81">
-        <v>77</v>
-      </c>
-      <c r="E8" s="41">
-        <v>1</v>
-      </c>
-      <c r="F8" s="42"/>
-      <c r="G8" s="41">
-        <v>1</v>
-      </c>
-      <c r="H8" s="41">
-        <v>640</v>
-      </c>
-      <c r="I8" s="41">
-        <v>480</v>
-      </c>
-      <c r="J8" s="41">
-        <v>5</v>
-      </c>
-      <c r="K8" s="41">
-        <v>5000</v>
-      </c>
-      <c r="L8" s="41">
-        <v>10</v>
-      </c>
-      <c r="M8" t="b" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="65"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="42"/>
-      <c r="M9" s="43"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="65"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="42"/>
-      <c r="M10" s="43"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="42"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="53"/>
-      <c r="M11" s="54"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3791,260 +4009,339 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="13.0859" style="82" customWidth="1"/>
-    <col min="2" max="2" width="9.72656" style="82" customWidth="1"/>
-    <col min="3" max="3" width="10.5391" style="82" customWidth="1"/>
-    <col min="4" max="11" width="9.72656" style="82" customWidth="1"/>
-    <col min="12" max="12" width="9.23438" style="82" customWidth="1"/>
-    <col min="13" max="16384" width="16.3516" style="82" customWidth="1"/>
+    <col min="2" max="3" width="9.72656" style="82" customWidth="1"/>
+    <col min="4" max="4" width="10.5391" style="82" customWidth="1"/>
+    <col min="5" max="14" width="9.72656" style="82" customWidth="1"/>
+    <col min="15" max="15" width="9.23438" style="82" customWidth="1"/>
+    <col min="16" max="16384" width="16.3516" style="82" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="63">
-        <v>79</v>
-      </c>
-      <c r="B1" s="28"/>
+      <c r="A1" t="s" s="62">
+        <v>85</v>
+      </c>
+      <c r="B1" s="27"/>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
       <c r="I1" s="28"/>
       <c r="J1" s="28"/>
       <c r="K1" s="28"/>
-      <c r="L1" s="30"/>
+      <c r="L1" s="28"/>
+      <c r="M1" s="28"/>
+      <c r="N1" s="28"/>
+      <c r="O1" s="30"/>
     </row>
     <row r="2" ht="26.7" customHeight="1">
       <c r="A2" t="s" s="31">
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>80</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s" s="32">
-        <v>81</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s" s="32">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E2" t="s" s="32">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="F2" t="s" s="32">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="G2" t="s" s="32">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="H2" t="s" s="32">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="I2" t="s" s="32">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="J2" t="s" s="32">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="K2" t="s" s="32">
-        <v>89</v>
-      </c>
-      <c r="L2" t="s" s="33">
-        <v>90</v>
+        <v>95</v>
+      </c>
+      <c r="L2" t="s" s="32">
+        <v>96</v>
+      </c>
+      <c r="M2" t="s" s="32">
+        <v>97</v>
+      </c>
+      <c r="N2" t="s" s="32">
+        <v>98</v>
+      </c>
+      <c r="O2" t="s" s="33">
+        <v>99</v>
       </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>91</v>
-      </c>
-      <c r="B3" s="35">
+        <v>100</v>
+      </c>
+      <c r="B3" t="s" s="83">
+        <v>101</v>
+      </c>
+      <c r="C3" s="35">
         <v>30</v>
       </c>
-      <c r="C3" s="36">
+      <c r="D3" s="36">
         <v>1</v>
       </c>
-      <c r="D3" s="36">
+      <c r="E3" s="36">
         <v>0.0036</v>
       </c>
-      <c r="E3" s="36">
-        <f>1/B3/2</f>
+      <c r="F3" s="36">
+        <f>1/C3/2</f>
         <v>0.0166666666666667</v>
       </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
-      <c r="K3" s="37"/>
-      <c r="L3" s="38"/>
+      <c r="G3" s="84">
+        <f>E3*F3</f>
+        <v>6.00000000000001e-05</v>
+      </c>
+      <c r="H3" s="36">
+        <v>1</v>
+      </c>
+      <c r="I3" s="75"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="37"/>
     </row>
     <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="39">
-        <v>92</v>
-      </c>
-      <c r="B4" s="40">
+      <c r="A4" t="s" s="38">
+        <v>102</v>
+      </c>
+      <c r="B4" t="s" s="85">
+        <v>101</v>
+      </c>
+      <c r="C4" s="39">
         <v>60</v>
       </c>
-      <c r="C4" s="41">
+      <c r="D4" s="40">
         <v>1</v>
       </c>
-      <c r="D4" s="41">
+      <c r="E4" s="40">
         <v>0.5</v>
       </c>
-      <c r="E4" s="41">
-        <f>1/B4/2</f>
+      <c r="F4" s="40">
+        <f>1/C4/2</f>
         <v>0.00833333333333333</v>
       </c>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="43"/>
+      <c r="G4" s="86">
+        <f>E4*F4</f>
+        <v>0.00416666666666667</v>
+      </c>
+      <c r="H4" s="40">
+        <v>1</v>
+      </c>
+      <c r="I4" s="41"/>
+      <c r="J4" s="41"/>
+      <c r="K4" s="41"/>
+      <c r="L4" s="41"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="42"/>
     </row>
     <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="39">
-        <v>93</v>
-      </c>
-      <c r="B5" s="40">
+      <c r="A5" t="s" s="38">
+        <v>103</v>
+      </c>
+      <c r="B5" t="s" s="85">
+        <v>101</v>
+      </c>
+      <c r="C5" s="39">
         <v>30</v>
       </c>
-      <c r="C5" s="41">
+      <c r="D5" s="40">
         <v>20000</v>
       </c>
-      <c r="D5" s="41">
-        <v>0.0036</v>
-      </c>
-      <c r="E5" s="41">
-        <f>1/B5/10</f>
-        <v>0.00333333333333333</v>
-      </c>
-      <c r="F5" s="83">
+      <c r="E5" s="40">
+        <v>0.03</v>
+      </c>
+      <c r="F5" s="40">
+        <v>0.004</v>
+      </c>
+      <c r="G5" s="86">
+        <f>E5*F5</f>
+        <v>0.00012</v>
+      </c>
+      <c r="H5" s="86">
+        <v>9</v>
+      </c>
+      <c r="I5" s="86">
         <v>3</v>
       </c>
-      <c r="G5" s="83">
+      <c r="J5" s="86">
         <v>3</v>
       </c>
-      <c r="H5" s="84">
+      <c r="K5" s="87">
         <v>10</v>
       </c>
-      <c r="I5" s="83">
+      <c r="L5" s="86">
         <v>1</v>
       </c>
-      <c r="J5" s="83">
+      <c r="M5" s="86">
         <v>1</v>
       </c>
-      <c r="K5" s="84">
+      <c r="N5" s="87">
         <v>8</v>
       </c>
-      <c r="L5" s="85">
+      <c r="O5" s="88">
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="39">
-        <v>94</v>
-      </c>
-      <c r="B6" s="40">
+      <c r="A6" t="s" s="38">
+        <v>104</v>
+      </c>
+      <c r="B6" t="s" s="85">
+        <v>101</v>
+      </c>
+      <c r="C6" s="39">
         <v>30</v>
       </c>
-      <c r="C6" s="41">
+      <c r="D6" s="40">
         <v>1</v>
       </c>
-      <c r="D6" s="41">
+      <c r="E6" s="40">
         <v>1</v>
       </c>
-      <c r="E6" s="41">
+      <c r="F6" s="40">
         <v>0.0001</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="43"/>
+      <c r="G6" s="86">
+        <f>E6*F6</f>
+        <v>0.0001</v>
+      </c>
+      <c r="H6" s="40">
+        <v>9</v>
+      </c>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="41"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="42"/>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="65"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="42"/>
-      <c r="K7" s="42"/>
-      <c r="L7" s="43"/>
+      <c r="A7" t="s" s="38">
+        <v>105</v>
+      </c>
+      <c r="B7" t="s" s="85">
+        <v>106</v>
+      </c>
+      <c r="C7" s="39">
+        <v>60</v>
+      </c>
+      <c r="D7" s="41"/>
+      <c r="E7" s="40">
+        <v>1</v>
+      </c>
+      <c r="F7" s="40">
+        <f>1/60/300/400</f>
+        <v>1.38888888888889e-07</v>
+      </c>
+      <c r="G7" s="86"/>
+      <c r="H7" s="40">
+        <v>1</v>
+      </c>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="41"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="42"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="65"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="42"/>
-      <c r="J8" s="42"/>
-      <c r="K8" s="42"/>
-      <c r="L8" s="43"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="89"/>
+      <c r="C8" s="65"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
+      <c r="G8" s="41"/>
+      <c r="H8" s="41"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="41"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="42"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="65"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
-      <c r="G9" s="42"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="42"/>
-      <c r="J9" s="42"/>
-      <c r="K9" s="42"/>
-      <c r="L9" s="43"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="89"/>
+      <c r="C9" s="65"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="41"/>
+      <c r="H9" s="41"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="41"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="42"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="65"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
-      <c r="G10" s="42"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="42"/>
-      <c r="J10" s="42"/>
-      <c r="K10" s="42"/>
-      <c r="L10" s="43"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="89"/>
+      <c r="C10" s="65"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="41"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="42"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="53"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="53"/>
-      <c r="L11" s="54"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="90"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="A1:O1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -4065,13 +4362,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="86" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="86" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="91" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="91" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="63">
-        <v>96</v>
+      <c r="A1" t="s" s="62">
+        <v>108</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -4083,104 +4380,80 @@
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>52</v>
-      </c>
-      <c r="C2" t="s" s="32">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s" s="32">
-        <v>53</v>
-      </c>
-      <c r="E2" t="s" s="33">
-        <v>54</v>
-      </c>
+        <v>109</v>
+      </c>
+      <c r="C2" s="32"/>
+      <c r="D2" s="92"/>
+      <c r="E2" s="63"/>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>97</v>
-      </c>
-      <c r="B3" s="35">
-        <v>2</v>
-      </c>
-      <c r="C3" s="36">
-        <v>0.9</v>
-      </c>
-      <c r="D3" s="70">
-        <v>0.005</v>
-      </c>
-      <c r="E3" s="71">
-        <v>50</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="B3" s="93"/>
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="37"/>
     </row>
     <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="39">
-        <v>98</v>
-      </c>
-      <c r="B4" s="40">
-        <v>2.4</v>
-      </c>
-      <c r="C4" s="41">
-        <v>0.9</v>
-      </c>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="A4" t="s" s="38">
+        <v>111</v>
+      </c>
+      <c r="B4" s="65"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
     </row>
     <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="39">
-        <v>99</v>
-      </c>
-      <c r="B5" s="40">
-        <v>1.4</v>
-      </c>
-      <c r="C5" s="41">
-        <v>0.9</v>
-      </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="45">
-        <v>50</v>
-      </c>
+      <c r="A5" t="s" s="38">
+        <v>112</v>
+      </c>
+      <c r="B5" s="65"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="42"/>
     </row>
     <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" s="65"/>
-      <c r="B6" s="66"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
+      <c r="A6" s="64"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="42"/>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" s="65"/>
-      <c r="B7" s="66"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="43"/>
+      <c r="A7" s="64"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="42"/>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" s="65"/>
-      <c r="B8" s="66"/>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="43"/>
+      <c r="A8" s="64"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="41"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="42"/>
     </row>
     <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" s="65"/>
-      <c r="B9" s="66"/>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="43"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="42"/>
     </row>
     <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" s="65"/>
-      <c r="B10" s="66"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="43"/>
+      <c r="A10" s="64"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="42"/>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" s="67"/>
-      <c r="B11" s="68"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="53"/>
-      <c r="E11" s="54"/>
+      <c r="A11" s="66"/>
+      <c r="B11" s="67"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="53"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -4199,19 +4472,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="87" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="87" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="94" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="94" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
-      <c r="A1" t="s" s="63">
-        <v>100</v>
+      <c r="A1" t="s" s="62">
+        <v>113</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -4241,222 +4514,242 @@
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>101</v>
-      </c>
-      <c r="B3" t="s" s="88">
+        <v>114</v>
+      </c>
+      <c r="B3" t="s" s="95">
         <v>29</v>
       </c>
-      <c r="C3" t="s" s="89">
-        <v>46</v>
-      </c>
-      <c r="D3" t="s" s="75">
-        <v>55</v>
-      </c>
-      <c r="E3" t="s" s="89">
-        <v>71</v>
-      </c>
-      <c r="F3" t="s" s="90">
-        <v>91</v>
+      <c r="C3" t="s" s="96">
+        <v>48</v>
+      </c>
+      <c r="D3" t="s" s="74">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s" s="96">
+        <v>76</v>
+      </c>
+      <c r="F3" t="s" s="97">
+        <v>100</v>
       </c>
     </row>
     <row r="4" ht="20.2" customHeight="1">
-      <c r="A4" t="s" s="39">
+      <c r="A4" t="s" s="38">
+        <v>115</v>
+      </c>
+      <c r="B4" t="s" s="98">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s" s="99">
+        <v>51</v>
+      </c>
+      <c r="D4" t="s" s="81">
+        <v>59</v>
+      </c>
+      <c r="E4" t="s" s="99">
+        <v>78</v>
+      </c>
+      <c r="F4" t="s" s="100">
         <v>102</v>
       </c>
-      <c r="B4" t="s" s="91">
-        <v>30</v>
-      </c>
-      <c r="C4" t="s" s="92">
-        <v>48</v>
-      </c>
-      <c r="D4" t="s" s="81">
-        <v>56</v>
-      </c>
-      <c r="E4" t="s" s="92">
-        <v>73</v>
-      </c>
-      <c r="F4" t="s" s="93">
-        <v>92</v>
-      </c>
     </row>
     <row r="5" ht="20.2" customHeight="1">
-      <c r="A5" t="s" s="39">
+      <c r="A5" t="s" s="38">
+        <v>116</v>
+      </c>
+      <c r="B5" t="s" s="98">
+        <v>29</v>
+      </c>
+      <c r="C5" t="s" s="99">
+        <v>53</v>
+      </c>
+      <c r="D5" t="s" s="81">
+        <v>60</v>
+      </c>
+      <c r="E5" t="s" s="99">
+        <v>76</v>
+      </c>
+      <c r="F5" t="s" s="100">
         <v>103</v>
       </c>
-      <c r="B5" t="s" s="91">
-        <v>29</v>
-      </c>
-      <c r="C5" t="s" s="92">
+    </row>
+    <row r="6" ht="20.2" customHeight="1">
+      <c r="A6" t="s" s="38">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s" s="101">
+        <v>35</v>
+      </c>
+      <c r="C6" t="s" s="99">
         <v>50</v>
       </c>
-      <c r="D5" t="s" s="81">
-        <v>57</v>
-      </c>
-      <c r="E5" t="s" s="92">
-        <v>71</v>
-      </c>
-      <c r="F5" t="s" s="93">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="6" ht="20.2" customHeight="1">
-      <c r="A6" t="s" s="94">
+      <c r="D6" t="s" s="99">
+        <v>61</v>
+      </c>
+      <c r="E6" t="s" s="99">
+        <v>84</v>
+      </c>
+      <c r="F6" t="s" s="100">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" ht="20.2" customHeight="1">
+      <c r="A7" t="s" s="102">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s" s="103">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s" s="38">
+        <v>53</v>
+      </c>
+      <c r="D7" t="s" s="98">
+        <v>60</v>
+      </c>
+      <c r="E7" t="s" s="104">
+        <v>79</v>
+      </c>
+      <c r="F7" t="s" s="100">
         <v>104</v>
       </c>
-      <c r="B6" t="s" s="95">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s" s="39">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s" s="91">
-        <v>57</v>
-      </c>
-      <c r="E6" t="s" s="96">
-        <v>74</v>
-      </c>
-      <c r="F6" t="s" s="93">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" t="s" s="39">
-        <v>105</v>
-      </c>
-      <c r="B7" t="s" s="97">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s" s="39">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s" s="91">
-        <v>57</v>
-      </c>
-      <c r="E7" t="s" s="96">
-        <v>75</v>
-      </c>
-      <c r="F7" t="s" s="93">
-        <v>94</v>
-      </c>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" t="s" s="39">
-        <v>106</v>
-      </c>
-      <c r="B8" t="s" s="98">
+      <c r="A8" t="s" s="38">
+        <v>119</v>
+      </c>
+      <c r="B8" t="s" s="105">
+        <v>41</v>
+      </c>
+      <c r="C8" t="s" s="38">
+        <v>53</v>
+      </c>
+      <c r="D8" t="s" s="98">
+        <v>60</v>
+      </c>
+      <c r="E8" t="s" s="104">
+        <v>80</v>
+      </c>
+      <c r="F8" t="s" s="100">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" ht="20.2" customHeight="1">
+      <c r="A9" t="s" s="38">
+        <v>120</v>
+      </c>
+      <c r="B9" t="s" s="106">
+        <v>42</v>
+      </c>
+      <c r="C9" t="s" s="38">
+        <v>53</v>
+      </c>
+      <c r="D9" t="s" s="98">
+        <v>60</v>
+      </c>
+      <c r="E9" t="s" s="104">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s" s="100">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" ht="20.2" customHeight="1">
+      <c r="A10" t="s" s="38">
+        <v>121</v>
+      </c>
+      <c r="B10" t="s" s="106">
+        <v>43</v>
+      </c>
+      <c r="C10" t="s" s="38">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s" s="98">
+        <v>60</v>
+      </c>
+      <c r="E10" t="s" s="104">
+        <v>83</v>
+      </c>
+      <c r="F10" t="s" s="100">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" ht="20.2" customHeight="1">
+      <c r="A11" t="s" s="102">
+        <v>122</v>
+      </c>
+      <c r="B11" t="s" s="103">
         <v>40</v>
       </c>
-      <c r="C8" t="s" s="39">
-        <v>50</v>
-      </c>
-      <c r="D8" t="s" s="91">
-        <v>57</v>
-      </c>
-      <c r="E8" t="s" s="96">
-        <v>76</v>
-      </c>
-      <c r="F8" t="s" s="93">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="9" ht="20.2" customHeight="1">
-      <c r="A9" t="s" s="39">
-        <v>107</v>
-      </c>
-      <c r="B9" t="s" s="98">
+      <c r="C11" t="s" s="38">
+        <v>52</v>
+      </c>
+      <c r="D11" t="s" s="98">
+        <v>60</v>
+      </c>
+      <c r="E11" t="s" s="104">
+        <v>79</v>
+      </c>
+      <c r="F11" t="s" s="100">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" ht="20.2" customHeight="1">
+      <c r="A12" t="s" s="38">
+        <v>123</v>
+      </c>
+      <c r="B12" t="s" s="105">
         <v>41</v>
       </c>
-      <c r="C9" t="s" s="39">
-        <v>50</v>
-      </c>
-      <c r="D9" t="s" s="91">
-        <v>57</v>
-      </c>
-      <c r="E9" t="s" s="96">
-        <v>78</v>
-      </c>
-      <c r="F9" t="s" s="93">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="10" ht="20.2" customHeight="1">
-      <c r="A10" t="s" s="94">
-        <v>108</v>
-      </c>
-      <c r="B10" t="s" s="95">
-        <v>38</v>
-      </c>
-      <c r="C10" t="s" s="39">
-        <v>49</v>
-      </c>
-      <c r="D10" t="s" s="91">
-        <v>57</v>
-      </c>
-      <c r="E10" t="s" s="96">
-        <v>74</v>
-      </c>
-      <c r="F10" t="s" s="93">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" t="s" s="39">
-        <v>109</v>
-      </c>
-      <c r="B11" t="s" s="97">
-        <v>39</v>
-      </c>
-      <c r="C11" t="s" s="39">
-        <v>49</v>
-      </c>
-      <c r="D11" t="s" s="91">
-        <v>57</v>
-      </c>
-      <c r="E11" t="s" s="96">
-        <v>75</v>
-      </c>
-      <c r="F11" t="s" s="93">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="12" ht="20.2" customHeight="1">
-      <c r="A12" t="s" s="39">
-        <v>110</v>
-      </c>
-      <c r="B12" t="s" s="98">
-        <v>40</v>
-      </c>
-      <c r="C12" t="s" s="39">
-        <v>49</v>
-      </c>
-      <c r="D12" t="s" s="91">
-        <v>57</v>
-      </c>
-      <c r="E12" t="s" s="96">
-        <v>76</v>
-      </c>
-      <c r="F12" t="s" s="93">
-        <v>94</v>
+      <c r="C12" t="s" s="38">
+        <v>52</v>
+      </c>
+      <c r="D12" t="s" s="98">
+        <v>60</v>
+      </c>
+      <c r="E12" t="s" s="104">
+        <v>80</v>
+      </c>
+      <c r="F12" t="s" s="100">
+        <v>104</v>
       </c>
     </row>
     <row r="13" ht="20.2" customHeight="1">
-      <c r="A13" t="s" s="39">
-        <v>111</v>
-      </c>
-      <c r="B13" t="s" s="98">
-        <v>41</v>
-      </c>
-      <c r="C13" t="s" s="39">
-        <v>49</v>
-      </c>
-      <c r="D13" t="s" s="91">
-        <v>57</v>
-      </c>
-      <c r="E13" t="s" s="96">
-        <v>78</v>
-      </c>
-      <c r="F13" t="s" s="93">
-        <v>94</v>
+      <c r="A13" t="s" s="38">
+        <v>124</v>
+      </c>
+      <c r="B13" t="s" s="106">
+        <v>42</v>
+      </c>
+      <c r="C13" t="s" s="38">
+        <v>52</v>
+      </c>
+      <c r="D13" t="s" s="98">
+        <v>60</v>
+      </c>
+      <c r="E13" t="s" s="104">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s" s="100">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" ht="20.2" customHeight="1">
+      <c r="A14" t="s" s="38">
+        <v>125</v>
+      </c>
+      <c r="B14" t="s" s="106">
+        <v>43</v>
+      </c>
+      <c r="C14" t="s" s="38">
+        <v>52</v>
+      </c>
+      <c r="D14" t="s" s="98">
+        <v>60</v>
+      </c>
+      <c r="E14" t="s" s="104">
+        <v>83</v>
+      </c>
+      <c r="F14" t="s" s="100">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Two LiDAR mode were inserted for flux test
</commit_message>
<xml_diff>
--- a/data/photonic_simul_data.xlsx
+++ b/data/photonic_simul_data.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="129">
   <si>
     <t>This document was exported from Numbers.  Each table was converted to an Excel worksheet. All other objects on each Numbers sheet were placed on separate worksheets. Please be aware that formula calculations may differ in Excel.</t>
   </si>
@@ -217,6 +217,20 @@
     </r>
   </si>
   <si>
+    <t>QLD_940_100S</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <u val="single"/>
+        <sz val="10"/>
+        <color indexed="12"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>http://www.qphotonics.com/Single-mode-laser-diode-100mW-940nm-QLD-940-100S.html</t>
+    </r>
+  </si>
+  <si>
     <t>MCM-124</t>
   </si>
   <si>
@@ -452,6 +466,9 @@
   </si>
   <si>
     <t>Lidar_2_axes</t>
+  </si>
+  <si>
+    <t>Lidar_2_axes_2</t>
   </si>
   <si>
     <t>fake_tof_night_850</t>
@@ -1078,13 +1095,13 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="8"/>
+        <color indexed="16"/>
       </left>
       <right style="thin">
-        <color indexed="8"/>
+        <color indexed="16"/>
       </right>
       <top style="thin">
-        <color indexed="8"/>
+        <color indexed="18"/>
       </top>
       <bottom style="thin">
         <color indexed="18"/>
@@ -1099,7 +1116,7 @@
         <color indexed="8"/>
       </right>
       <top style="thin">
-        <color indexed="18"/>
+        <color indexed="8"/>
       </top>
       <bottom style="thin">
         <color indexed="18"/>
@@ -1117,22 +1134,22 @@
         <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="16"/>
+        <color indexed="18"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="16"/>
+        <color indexed="8"/>
       </left>
       <right style="thin">
-        <color indexed="16"/>
+        <color indexed="8"/>
       </right>
       <top style="thin">
         <color indexed="18"/>
       </top>
       <bottom style="thin">
-        <color indexed="18"/>
+        <color indexed="16"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1187,7 +1204,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="108">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1434,16 +1451,19 @@
     <xf numFmtId="49" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="61" fontId="0" fillId="6" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="6" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="61" fontId="0" fillId="6" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1455,12 +1475,12 @@
     <xf numFmtId="61" fontId="0" fillId="6" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="39" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="40" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="41" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1494,7 +1514,7 @@
     <xf numFmtId="49" fontId="7" fillId="6" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="8" borderId="41" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="7" fillId="8" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -2803,7 +2823,7 @@
     </row>
     <row r="21">
       <c r="B21" t="s" s="3">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -2814,7 +2834,7 @@
         <v>5</v>
       </c>
       <c r="D22" t="s" s="5">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23">
@@ -2864,7 +2884,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:J16"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -3112,70 +3132,75 @@
         <v>39</v>
       </c>
       <c r="B9" s="39">
-        <v>28</v>
-      </c>
-      <c r="C9" s="46">
-        <v>1375</v>
+        <v>0.1</v>
+      </c>
+      <c r="C9" s="40">
+        <v>940</v>
       </c>
       <c r="D9" s="40">
         <v>0.95</v>
       </c>
       <c r="E9" s="40">
+        <v>0.1</v>
+      </c>
+      <c r="F9" s="44">
+        <v>0.1</v>
+      </c>
+      <c r="G9" s="45">
+        <v>1</v>
+      </c>
+      <c r="H9" s="40">
+        <v>1.63</v>
+      </c>
+      <c r="I9" s="40">
+        <v>0.137</v>
+      </c>
+      <c r="J9" t="s" s="43">
         <v>40</v>
-      </c>
-      <c r="F9" s="40">
-        <v>20</v>
-      </c>
-      <c r="G9" s="40">
-        <v>1</v>
-      </c>
-      <c r="H9" s="40">
-        <v>11.5</v>
-      </c>
-      <c r="I9" s="40">
-        <v>12.5</v>
-      </c>
-      <c r="J9" t="s" s="43">
-        <v>34</v>
       </c>
     </row>
     <row r="10" ht="20.2" customHeight="1">
       <c r="A10" t="s" s="38">
+        <v>41</v>
+      </c>
+      <c r="B10" s="39">
+        <v>28</v>
+      </c>
+      <c r="C10" s="46">
+        <v>1375</v>
+      </c>
+      <c r="D10" s="40">
+        <v>0.95</v>
+      </c>
+      <c r="E10" s="40">
         <v>40</v>
       </c>
-      <c r="B10" s="39">
+      <c r="F10" s="40">
+        <v>20</v>
+      </c>
+      <c r="G10" s="40">
+        <v>1</v>
+      </c>
+      <c r="H10" s="40">
+        <v>11.5</v>
+      </c>
+      <c r="I10" s="40">
+        <v>12.5</v>
+      </c>
+      <c r="J10" t="s" s="43">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" ht="20.2" customHeight="1">
+      <c r="A11" t="s" s="38">
+        <v>42</v>
+      </c>
+      <c r="B11" s="39">
         <f>50*0.5</f>
         <v>25</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C11" s="36">
         <v>850</v>
-      </c>
-      <c r="D10" s="40">
-        <v>0.95</v>
-      </c>
-      <c r="E10" s="40">
-        <v>70</v>
-      </c>
-      <c r="F10" s="40">
-        <v>60</v>
-      </c>
-      <c r="G10" s="40">
-        <v>2</v>
-      </c>
-      <c r="H10" s="41"/>
-      <c r="I10" s="41"/>
-      <c r="J10" s="42"/>
-    </row>
-    <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" t="s" s="47">
-        <v>41</v>
-      </c>
-      <c r="B11" s="39">
-        <f>50*0.38</f>
-        <v>19</v>
-      </c>
-      <c r="C11" s="40">
-        <v>940</v>
       </c>
       <c r="D11" s="40">
         <v>0.95</v>
@@ -3194,15 +3219,15 @@
       <c r="J11" s="42"/>
     </row>
     <row r="12" ht="20.2" customHeight="1">
-      <c r="A12" t="s" s="48">
-        <v>42</v>
+      <c r="A12" t="s" s="47">
+        <v>43</v>
       </c>
       <c r="B12" s="39">
-        <f>50*0.22</f>
-        <v>11</v>
+        <f>50*0.38</f>
+        <v>19</v>
       </c>
       <c r="C12" s="40">
-        <v>1375</v>
+        <v>940</v>
       </c>
       <c r="D12" s="40">
         <v>0.95</v>
@@ -3221,55 +3246,82 @@
       <c r="J12" s="42"/>
     </row>
     <row r="13" ht="20.2" customHeight="1">
-      <c r="A13" t="s" s="49">
-        <v>43</v>
-      </c>
-      <c r="B13" s="50">
-        <f>50*0.19+C15</f>
+      <c r="A13" t="s" s="48">
+        <v>44</v>
+      </c>
+      <c r="B13" s="39">
+        <f>50*0.22</f>
+        <v>11</v>
+      </c>
+      <c r="C13" s="40">
+        <v>1375</v>
+      </c>
+      <c r="D13" s="40">
+        <v>0.95</v>
+      </c>
+      <c r="E13" s="40">
+        <v>70</v>
+      </c>
+      <c r="F13" s="40">
+        <v>60</v>
+      </c>
+      <c r="G13" s="40">
+        <v>2</v>
+      </c>
+      <c r="H13" s="41"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="42"/>
+    </row>
+    <row r="14" ht="20.2" customHeight="1">
+      <c r="A14" t="s" s="49">
+        <v>45</v>
+      </c>
+      <c r="B14" s="50">
+        <f>50*0.19+C16</f>
         <v>9.5</v>
       </c>
-      <c r="C13" s="40">
+      <c r="C14" s="40">
         <v>1550</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D14" s="51">
         <v>0.95</v>
       </c>
-      <c r="E13" s="51">
+      <c r="E14" s="51">
         <v>70</v>
       </c>
-      <c r="F13" s="51">
+      <c r="F14" s="51">
         <v>60</v>
       </c>
-      <c r="G13" s="51">
+      <c r="G14" s="51">
         <v>2</v>
       </c>
-      <c r="H13" s="52"/>
-      <c r="I13" s="52"/>
-      <c r="J13" s="53"/>
-    </row>
-    <row r="14" ht="14.7" customHeight="1">
-      <c r="A14" s="54"/>
-      <c r="B14" s="55"/>
-      <c r="C14" s="56"/>
-      <c r="D14" s="55"/>
-      <c r="E14" s="55"/>
-      <c r="F14" s="55"/>
-      <c r="G14" s="55"/>
-      <c r="H14" s="55"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="57"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="53"/>
     </row>
     <row r="15" ht="14.7" customHeight="1">
-      <c r="A15" s="58"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="59"/>
-      <c r="E15" s="59"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="60"/>
+      <c r="A15" s="54"/>
+      <c r="B15" s="55"/>
+      <c r="C15" s="56"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="55"/>
+      <c r="F15" s="55"/>
+      <c r="G15" s="55"/>
+      <c r="H15" s="55"/>
+      <c r="I15" s="55"/>
+      <c r="J15" s="57"/>
+    </row>
+    <row r="16" ht="14.7" customHeight="1">
+      <c r="A16" s="58"/>
+      <c r="B16" s="59"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="59"/>
+      <c r="F16" s="59"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="59"/>
+      <c r="J16" s="60"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -3277,7 +3329,8 @@
     <hyperlink ref="J6" r:id="rId2" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
     <hyperlink ref="J7" r:id="rId3" location="" tooltip="" display="https://www.ii-vi.com/wp-content/uploads/2019/07/940nm-Multi-Mode-High-Power-VCSEL-Array-web-2-1.pdf"/>
     <hyperlink ref="J8" r:id="rId4" location="" tooltip="" display="https://www.osram.com/ecat/Metal%20Can%C2%AE%20TO56%20SPL%20UL90AT08/com/en/class_pim_web_catalog_103489/global/prd_pim_device_2220021/"/>
-    <hyperlink ref="J9" r:id="rId5" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
+    <hyperlink ref="J9" r:id="rId5" location="" tooltip="" display="http://www.qphotonics.com/Single-mode-laser-diode-100mW-940nm-QLD-940-100S.html"/>
+    <hyperlink ref="J10" r:id="rId6" location="" tooltip="" display="https://www.laserdiodesource.com/files/pdfs/laserdiodesource_com/product-2924/1550nm_20W_Fiber_Coupled_Module_Seminex-1459186218.pdf"/>
   </hyperlinks>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
@@ -3304,7 +3357,7 @@
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" t="s" s="62">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -3316,19 +3369,19 @@
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C2" t="s" s="32">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="D2" t="s" s="32">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="E2" s="63"/>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B3" s="35">
         <v>3</v>
@@ -3343,7 +3396,7 @@
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="38">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B4" s="39">
         <v>60</v>
@@ -3358,7 +3411,7 @@
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="38">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B5" s="39">
         <v>200</v>
@@ -3373,7 +3426,7 @@
     </row>
     <row r="6" ht="20.2" customHeight="1">
       <c r="A6" t="s" s="38">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B6" s="39">
         <v>200</v>
@@ -3388,7 +3441,7 @@
     </row>
     <row r="7" ht="20.2" customHeight="1">
       <c r="A7" t="s" s="38">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B7" s="39">
         <v>5</v>
@@ -3403,7 +3456,7 @@
     </row>
     <row r="8" ht="20.2" customHeight="1">
       <c r="A8" t="s" s="38">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B8" s="39">
         <v>5</v>
@@ -3473,7 +3526,7 @@
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" t="s" s="62">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -3485,21 +3538,21 @@
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s" s="32">
         <v>22</v>
       </c>
       <c r="D2" t="s" s="32">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s" s="33">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B3" s="35">
         <v>2</v>
@@ -3516,7 +3569,7 @@
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="38">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B4" s="39">
         <v>2.4</v>
@@ -3529,7 +3582,7 @@
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="38">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B5" s="39">
         <v>1.4</v>
@@ -3544,7 +3597,7 @@
     </row>
     <row r="6" ht="20.2" customHeight="1">
       <c r="A6" t="s" s="38">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B6" s="39">
         <v>1</v>
@@ -3623,7 +3676,7 @@
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" s="26"/>
       <c r="B1" t="s" s="29">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="27"/>
@@ -3643,48 +3696,48 @@
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="C2" t="s" s="32">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="D2" t="s" s="32">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E2" t="s" s="32">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="F2" t="s" s="32">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s" s="32">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="H2" t="s" s="32">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="I2" t="s" s="32">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="J2" t="s" s="32">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="K2" t="s" s="32">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="L2" t="s" s="32">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="M2" t="s" s="32">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="N2" t="s" s="33">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B3" s="73">
         <v>7</v>
@@ -3693,7 +3746,7 @@
         <v>850</v>
       </c>
       <c r="D3" t="s" s="74">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E3" s="36">
         <v>10</v>
@@ -3724,7 +3777,7 @@
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="76">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B4" s="77">
         <v>3</v>
@@ -3733,7 +3786,7 @@
         <v>550</v>
       </c>
       <c r="D4" t="s" s="78">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E4" s="46">
         <v>10</v>
@@ -3764,7 +3817,7 @@
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="34">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B5" s="35">
         <v>7.5</v>
@@ -3773,7 +3826,7 @@
         <v>850</v>
       </c>
       <c r="D5" t="s" s="74">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E5" s="36">
         <v>10</v>
@@ -3806,7 +3859,7 @@
     </row>
     <row r="6" ht="20.2" customHeight="1">
       <c r="A6" t="s" s="38">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B6" s="39">
         <v>7.5</v>
@@ -3815,7 +3868,7 @@
         <v>940</v>
       </c>
       <c r="D6" t="s" s="81">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E6" s="40">
         <v>10</v>
@@ -3848,7 +3901,7 @@
     </row>
     <row r="7" ht="20.2" customHeight="1">
       <c r="A7" t="s" s="38">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B7" s="39">
         <v>7.5</v>
@@ -3857,7 +3910,7 @@
         <v>1375</v>
       </c>
       <c r="D7" t="s" s="81">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E7" s="40">
         <v>1</v>
@@ -3890,7 +3943,7 @@
     </row>
     <row r="8" ht="20.2" customHeight="1">
       <c r="A8" t="s" s="38">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B8" s="39">
         <v>7.5</v>
@@ -3899,7 +3952,7 @@
         <v>1550</v>
       </c>
       <c r="D8" t="s" s="81">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E8" s="40">
         <v>1</v>
@@ -3932,7 +3985,7 @@
     </row>
     <row r="9" ht="20.2" customHeight="1">
       <c r="A9" t="s" s="38">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B9" s="39">
         <v>20</v>
@@ -3941,7 +3994,7 @@
         <v>940</v>
       </c>
       <c r="D9" t="s" s="81">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="E9" s="40">
         <v>30</v>
@@ -3950,13 +4003,25 @@
       <c r="G9" s="40">
         <v>1</v>
       </c>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
-      <c r="N9" s="44">
+      <c r="H9" s="40">
+        <v>400</v>
+      </c>
+      <c r="I9" s="40">
+        <v>300</v>
+      </c>
+      <c r="J9" s="40">
+        <v>5</v>
+      </c>
+      <c r="K9" s="40">
+        <v>5000</v>
+      </c>
+      <c r="L9" s="40">
+        <v>10</v>
+      </c>
+      <c r="M9" t="b" s="44">
+        <v>0</v>
+      </c>
+      <c r="N9" s="82">
         <v>10</v>
       </c>
     </row>
@@ -4015,17 +4080,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="13.0859" style="82" customWidth="1"/>
-    <col min="2" max="3" width="9.72656" style="82" customWidth="1"/>
-    <col min="4" max="4" width="10.5391" style="82" customWidth="1"/>
-    <col min="5" max="14" width="9.72656" style="82" customWidth="1"/>
-    <col min="15" max="15" width="9.23438" style="82" customWidth="1"/>
-    <col min="16" max="16384" width="16.3516" style="82" customWidth="1"/>
+    <col min="1" max="1" width="13.0859" style="83" customWidth="1"/>
+    <col min="2" max="3" width="9.72656" style="83" customWidth="1"/>
+    <col min="4" max="4" width="10.5391" style="83" customWidth="1"/>
+    <col min="5" max="14" width="9.72656" style="83" customWidth="1"/>
+    <col min="15" max="15" width="9.23438" style="83" customWidth="1"/>
+    <col min="16" max="16384" width="16.3516" style="83" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" t="s" s="62">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="28"/>
@@ -4047,54 +4112,54 @@
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s" s="32">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D2" t="s" s="32">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="E2" t="s" s="32">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="F2" t="s" s="32">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="G2" t="s" s="32">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="H2" t="s" s="32">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="I2" t="s" s="32">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J2" t="s" s="32">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K2" t="s" s="32">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="L2" t="s" s="32">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="M2" t="s" s="32">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="N2" t="s" s="32">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O2" t="s" s="33">
-        <v>99</v>
+        <v>101</v>
       </c>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>100</v>
-      </c>
-      <c r="B3" t="s" s="83">
-        <v>101</v>
+        <v>102</v>
+      </c>
+      <c r="B3" t="s" s="84">
+        <v>103</v>
       </c>
       <c r="C3" s="35">
         <v>30</v>
@@ -4109,7 +4174,7 @@
         <f>1/C3/2</f>
         <v>0.0166666666666667</v>
       </c>
-      <c r="G3" s="84">
+      <c r="G3" s="85">
         <f>E3*F3</f>
         <v>6.00000000000001e-05</v>
       </c>
@@ -4126,10 +4191,10 @@
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="38">
-        <v>102</v>
-      </c>
-      <c r="B4" t="s" s="85">
-        <v>101</v>
+        <v>104</v>
+      </c>
+      <c r="B4" t="s" s="86">
+        <v>103</v>
       </c>
       <c r="C4" s="39">
         <v>60</v>
@@ -4144,7 +4209,7 @@
         <f>1/C4/2</f>
         <v>0.00833333333333333</v>
       </c>
-      <c r="G4" s="86">
+      <c r="G4" s="87">
         <f>E4*F4</f>
         <v>0.00416666666666667</v>
       </c>
@@ -4161,10 +4226,10 @@
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="38">
+        <v>105</v>
+      </c>
+      <c r="B5" t="s" s="86">
         <v>103</v>
-      </c>
-      <c r="B5" t="s" s="85">
-        <v>101</v>
       </c>
       <c r="C5" s="39">
         <v>30</v>
@@ -4178,41 +4243,41 @@
       <c r="F5" s="40">
         <v>0.004</v>
       </c>
-      <c r="G5" s="86">
+      <c r="G5" s="87">
         <f>E5*F5</f>
         <v>0.00012</v>
       </c>
-      <c r="H5" s="86">
+      <c r="H5" s="87">
         <v>9</v>
       </c>
-      <c r="I5" s="86">
+      <c r="I5" s="87">
         <v>3</v>
       </c>
-      <c r="J5" s="86">
+      <c r="J5" s="87">
         <v>3</v>
       </c>
-      <c r="K5" s="87">
+      <c r="K5" s="88">
         <v>10</v>
       </c>
-      <c r="L5" s="86">
+      <c r="L5" s="87">
         <v>1</v>
       </c>
-      <c r="M5" s="86">
+      <c r="M5" s="87">
         <v>1</v>
       </c>
-      <c r="N5" s="87">
+      <c r="N5" s="88">
         <v>8</v>
       </c>
-      <c r="O5" s="88">
+      <c r="O5" s="89">
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
       <c r="A6" t="s" s="38">
-        <v>104</v>
-      </c>
-      <c r="B6" t="s" s="85">
-        <v>101</v>
+        <v>106</v>
+      </c>
+      <c r="B6" t="s" s="86">
+        <v>103</v>
       </c>
       <c r="C6" s="39">
         <v>30</v>
@@ -4226,7 +4291,7 @@
       <c r="F6" s="40">
         <v>0.0001</v>
       </c>
-      <c r="G6" s="86">
+      <c r="G6" s="87">
         <f>E6*F6</f>
         <v>0.0001</v>
       </c>
@@ -4243,15 +4308,17 @@
     </row>
     <row r="7" ht="20.2" customHeight="1">
       <c r="A7" t="s" s="38">
-        <v>105</v>
-      </c>
-      <c r="B7" t="s" s="85">
-        <v>106</v>
+        <v>107</v>
+      </c>
+      <c r="B7" t="s" s="86">
+        <v>108</v>
       </c>
       <c r="C7" s="39">
         <v>60</v>
       </c>
-      <c r="D7" s="41"/>
+      <c r="D7" s="40">
+        <v>1</v>
+      </c>
       <c r="E7" s="40">
         <v>1</v>
       </c>
@@ -4259,7 +4326,10 @@
         <f>1/60/300/400</f>
         <v>1.38888888888889e-07</v>
       </c>
-      <c r="G7" s="86"/>
+      <c r="G7" s="87">
+        <f>E7*F7</f>
+        <v>1.38888888888889e-07</v>
+      </c>
       <c r="H7" s="40">
         <v>1</v>
       </c>
@@ -4273,7 +4343,7 @@
     </row>
     <row r="8" ht="20.2" customHeight="1">
       <c r="A8" s="64"/>
-      <c r="B8" s="89"/>
+      <c r="B8" s="90"/>
       <c r="C8" s="65"/>
       <c r="D8" s="41"/>
       <c r="E8" s="41"/>
@@ -4290,7 +4360,7 @@
     </row>
     <row r="9" ht="20.2" customHeight="1">
       <c r="A9" s="64"/>
-      <c r="B9" s="89"/>
+      <c r="B9" s="90"/>
       <c r="C9" s="65"/>
       <c r="D9" s="41"/>
       <c r="E9" s="41"/>
@@ -4307,7 +4377,7 @@
     </row>
     <row r="10" ht="20.2" customHeight="1">
       <c r="A10" s="64"/>
-      <c r="B10" s="89"/>
+      <c r="B10" s="90"/>
       <c r="C10" s="65"/>
       <c r="D10" s="41"/>
       <c r="E10" s="41"/>
@@ -4324,7 +4394,7 @@
     </row>
     <row r="11" ht="20.2" customHeight="1">
       <c r="A11" s="66"/>
-      <c r="B11" s="90"/>
+      <c r="B11" s="91"/>
       <c r="C11" s="67"/>
       <c r="D11" s="52"/>
       <c r="E11" s="52"/>
@@ -4362,13 +4432,13 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="5" width="16.3516" style="91" customWidth="1"/>
-    <col min="6" max="16384" width="16.3516" style="91" customWidth="1"/>
+    <col min="1" max="5" width="16.3516" style="92" customWidth="1"/>
+    <col min="6" max="16384" width="16.3516" style="92" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" t="s" s="62">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -4380,24 +4450,24 @@
         <v>19</v>
       </c>
       <c r="B2" t="s" s="32">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="C2" s="32"/>
-      <c r="D2" s="92"/>
+      <c r="D2" s="93"/>
       <c r="E2" s="63"/>
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>110</v>
-      </c>
-      <c r="B3" s="93"/>
+        <v>112</v>
+      </c>
+      <c r="B3" s="94"/>
       <c r="C3" s="75"/>
       <c r="D3" s="75"/>
       <c r="E3" s="37"/>
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="38">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B4" s="65"/>
       <c r="C4" s="41"/>
@@ -4406,7 +4476,7 @@
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="38">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B5" s="65"/>
       <c r="C5" s="41"/>
@@ -4472,19 +4542,19 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="6" width="16.3516" style="94" customWidth="1"/>
-    <col min="7" max="16384" width="16.3516" style="94" customWidth="1"/>
+    <col min="1" max="6" width="16.3516" style="95" customWidth="1"/>
+    <col min="7" max="16384" width="16.3516" style="95" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="25.65" customHeight="1">
       <c r="A1" t="s" s="62">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -4514,242 +4584,262 @@
     </row>
     <row r="3" ht="20.45" customHeight="1">
       <c r="A3" t="s" s="34">
-        <v>114</v>
-      </c>
-      <c r="B3" t="s" s="95">
+        <v>116</v>
+      </c>
+      <c r="B3" t="s" s="96">
         <v>29</v>
       </c>
-      <c r="C3" t="s" s="96">
-        <v>48</v>
+      <c r="C3" t="s" s="97">
+        <v>50</v>
       </c>
       <c r="D3" t="s" s="74">
-        <v>58</v>
-      </c>
-      <c r="E3" t="s" s="96">
-        <v>76</v>
-      </c>
-      <c r="F3" t="s" s="97">
-        <v>100</v>
+        <v>60</v>
+      </c>
+      <c r="E3" t="s" s="97">
+        <v>78</v>
+      </c>
+      <c r="F3" t="s" s="98">
+        <v>102</v>
       </c>
     </row>
     <row r="4" ht="20.2" customHeight="1">
       <c r="A4" t="s" s="38">
-        <v>115</v>
-      </c>
-      <c r="B4" t="s" s="98">
+        <v>117</v>
+      </c>
+      <c r="B4" t="s" s="99">
         <v>30</v>
       </c>
-      <c r="C4" t="s" s="99">
-        <v>51</v>
+      <c r="C4" t="s" s="100">
+        <v>53</v>
       </c>
       <c r="D4" t="s" s="81">
-        <v>59</v>
-      </c>
-      <c r="E4" t="s" s="99">
-        <v>78</v>
-      </c>
-      <c r="F4" t="s" s="100">
-        <v>102</v>
+        <v>61</v>
+      </c>
+      <c r="E4" t="s" s="100">
+        <v>80</v>
+      </c>
+      <c r="F4" t="s" s="101">
+        <v>104</v>
       </c>
     </row>
     <row r="5" ht="20.2" customHeight="1">
       <c r="A5" t="s" s="38">
-        <v>116</v>
-      </c>
-      <c r="B5" t="s" s="98">
+        <v>118</v>
+      </c>
+      <c r="B5" t="s" s="99">
         <v>29</v>
       </c>
-      <c r="C5" t="s" s="99">
-        <v>53</v>
+      <c r="C5" t="s" s="100">
+        <v>55</v>
       </c>
       <c r="D5" t="s" s="81">
-        <v>60</v>
-      </c>
-      <c r="E5" t="s" s="99">
-        <v>76</v>
-      </c>
-      <c r="F5" t="s" s="100">
-        <v>103</v>
+        <v>62</v>
+      </c>
+      <c r="E5" t="s" s="100">
+        <v>78</v>
+      </c>
+      <c r="F5" t="s" s="101">
+        <v>105</v>
       </c>
     </row>
     <row r="6" ht="20.2" customHeight="1">
       <c r="A6" t="s" s="38">
-        <v>117</v>
-      </c>
-      <c r="B6" t="s" s="101">
-        <v>35</v>
-      </c>
-      <c r="C6" t="s" s="99">
-        <v>50</v>
-      </c>
-      <c r="D6" t="s" s="99">
-        <v>61</v>
-      </c>
-      <c r="E6" t="s" s="99">
-        <v>84</v>
-      </c>
-      <c r="F6" t="s" s="100">
-        <v>105</v>
+        <v>119</v>
+      </c>
+      <c r="B6" t="s" s="102">
+        <v>39</v>
+      </c>
+      <c r="C6" t="s" s="100">
+        <v>52</v>
+      </c>
+      <c r="D6" t="s" s="100">
+        <v>63</v>
+      </c>
+      <c r="E6" t="s" s="100">
+        <v>86</v>
+      </c>
+      <c r="F6" t="s" s="101">
+        <v>107</v>
       </c>
     </row>
     <row r="7" ht="20.2" customHeight="1">
-      <c r="A7" t="s" s="102">
-        <v>118</v>
-      </c>
-      <c r="B7" t="s" s="103">
-        <v>40</v>
-      </c>
-      <c r="C7" t="s" s="38">
-        <v>53</v>
-      </c>
-      <c r="D7" t="s" s="98">
-        <v>60</v>
-      </c>
-      <c r="E7" t="s" s="104">
-        <v>79</v>
-      </c>
-      <c r="F7" t="s" s="100">
-        <v>104</v>
+      <c r="A7" t="s" s="38">
+        <v>120</v>
+      </c>
+      <c r="B7" t="s" s="102">
+        <v>37</v>
+      </c>
+      <c r="C7" t="s" s="100">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s" s="100">
+        <v>63</v>
+      </c>
+      <c r="E7" t="s" s="100">
+        <v>86</v>
+      </c>
+      <c r="F7" t="s" s="101">
+        <v>107</v>
       </c>
     </row>
     <row r="8" ht="20.2" customHeight="1">
-      <c r="A8" t="s" s="38">
-        <v>119</v>
-      </c>
-      <c r="B8" t="s" s="105">
-        <v>41</v>
+      <c r="A8" t="s" s="103">
+        <v>121</v>
+      </c>
+      <c r="B8" t="s" s="104">
+        <v>42</v>
       </c>
       <c r="C8" t="s" s="38">
-        <v>53</v>
-      </c>
-      <c r="D8" t="s" s="98">
-        <v>60</v>
-      </c>
-      <c r="E8" t="s" s="104">
-        <v>80</v>
-      </c>
-      <c r="F8" t="s" s="100">
-        <v>104</v>
+        <v>55</v>
+      </c>
+      <c r="D8" t="s" s="99">
+        <v>62</v>
+      </c>
+      <c r="E8" t="s" s="105">
+        <v>81</v>
+      </c>
+      <c r="F8" t="s" s="101">
+        <v>106</v>
       </c>
     </row>
     <row r="9" ht="20.2" customHeight="1">
       <c r="A9" t="s" s="38">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B9" t="s" s="106">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C9" t="s" s="38">
-        <v>53</v>
-      </c>
-      <c r="D9" t="s" s="98">
-        <v>60</v>
-      </c>
-      <c r="E9" t="s" s="104">
-        <v>81</v>
-      </c>
-      <c r="F9" t="s" s="100">
-        <v>104</v>
+        <v>55</v>
+      </c>
+      <c r="D9" t="s" s="99">
+        <v>62</v>
+      </c>
+      <c r="E9" t="s" s="105">
+        <v>82</v>
+      </c>
+      <c r="F9" t="s" s="101">
+        <v>106</v>
       </c>
     </row>
     <row r="10" ht="20.2" customHeight="1">
       <c r="A10" t="s" s="38">
-        <v>121</v>
-      </c>
-      <c r="B10" t="s" s="106">
-        <v>43</v>
+        <v>123</v>
+      </c>
+      <c r="B10" t="s" s="107">
+        <v>44</v>
       </c>
       <c r="C10" t="s" s="38">
-        <v>53</v>
-      </c>
-      <c r="D10" t="s" s="98">
-        <v>60</v>
-      </c>
-      <c r="E10" t="s" s="104">
+        <v>55</v>
+      </c>
+      <c r="D10" t="s" s="99">
+        <v>62</v>
+      </c>
+      <c r="E10" t="s" s="105">
         <v>83</v>
       </c>
-      <c r="F10" t="s" s="100">
-        <v>104</v>
+      <c r="F10" t="s" s="101">
+        <v>106</v>
       </c>
     </row>
     <row r="11" ht="20.2" customHeight="1">
-      <c r="A11" t="s" s="102">
-        <v>122</v>
-      </c>
-      <c r="B11" t="s" s="103">
-        <v>40</v>
+      <c r="A11" t="s" s="38">
+        <v>124</v>
+      </c>
+      <c r="B11" t="s" s="107">
+        <v>45</v>
       </c>
       <c r="C11" t="s" s="38">
-        <v>52</v>
-      </c>
-      <c r="D11" t="s" s="98">
-        <v>60</v>
-      </c>
-      <c r="E11" t="s" s="104">
-        <v>79</v>
-      </c>
-      <c r="F11" t="s" s="100">
-        <v>104</v>
+        <v>55</v>
+      </c>
+      <c r="D11" t="s" s="99">
+        <v>62</v>
+      </c>
+      <c r="E11" t="s" s="105">
+        <v>85</v>
+      </c>
+      <c r="F11" t="s" s="101">
+        <v>106</v>
       </c>
     </row>
     <row r="12" ht="20.2" customHeight="1">
-      <c r="A12" t="s" s="38">
-        <v>123</v>
-      </c>
-      <c r="B12" t="s" s="105">
-        <v>41</v>
+      <c r="A12" t="s" s="103">
+        <v>125</v>
+      </c>
+      <c r="B12" t="s" s="104">
+        <v>42</v>
       </c>
       <c r="C12" t="s" s="38">
-        <v>52</v>
-      </c>
-      <c r="D12" t="s" s="98">
-        <v>60</v>
-      </c>
-      <c r="E12" t="s" s="104">
-        <v>80</v>
-      </c>
-      <c r="F12" t="s" s="100">
-        <v>104</v>
+        <v>54</v>
+      </c>
+      <c r="D12" t="s" s="99">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s" s="105">
+        <v>81</v>
+      </c>
+      <c r="F12" t="s" s="101">
+        <v>106</v>
       </c>
     </row>
     <row r="13" ht="20.2" customHeight="1">
       <c r="A13" t="s" s="38">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s" s="106">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C13" t="s" s="38">
-        <v>52</v>
-      </c>
-      <c r="D13" t="s" s="98">
-        <v>60</v>
-      </c>
-      <c r="E13" t="s" s="104">
-        <v>81</v>
-      </c>
-      <c r="F13" t="s" s="100">
-        <v>104</v>
+        <v>54</v>
+      </c>
+      <c r="D13" t="s" s="99">
+        <v>62</v>
+      </c>
+      <c r="E13" t="s" s="105">
+        <v>82</v>
+      </c>
+      <c r="F13" t="s" s="101">
+        <v>106</v>
       </c>
     </row>
     <row r="14" ht="20.2" customHeight="1">
       <c r="A14" t="s" s="38">
-        <v>125</v>
-      </c>
-      <c r="B14" t="s" s="106">
-        <v>43</v>
+        <v>127</v>
+      </c>
+      <c r="B14" t="s" s="107">
+        <v>44</v>
       </c>
       <c r="C14" t="s" s="38">
-        <v>52</v>
-      </c>
-      <c r="D14" t="s" s="98">
-        <v>60</v>
-      </c>
-      <c r="E14" t="s" s="104">
+        <v>54</v>
+      </c>
+      <c r="D14" t="s" s="99">
+        <v>62</v>
+      </c>
+      <c r="E14" t="s" s="105">
         <v>83</v>
       </c>
-      <c r="F14" t="s" s="100">
-        <v>104</v>
+      <c r="F14" t="s" s="101">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" ht="20.2" customHeight="1">
+      <c r="A15" t="s" s="38">
+        <v>128</v>
+      </c>
+      <c r="B15" t="s" s="107">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s" s="38">
+        <v>54</v>
+      </c>
+      <c r="D15" t="s" s="99">
+        <v>62</v>
+      </c>
+      <c r="E15" t="s" s="105">
+        <v>85</v>
+      </c>
+      <c r="F15" t="s" s="101">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>